<commit_message>
Added test cases for studentbreakdown
</commit_message>
<xml_diff>
--- a/testing/Testcases-iteration.xlsx
+++ b/testing/Testcases-iteration.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amanda\Desktop\SE\SE\is203-2017_G1T3\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User-PC\Documents\is203-2017_G1T3\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" tabRatio="1000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" tabRatio="1000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case for Login Validation" sheetId="1" r:id="rId1"/>
     <sheet name="Test Case for Bootstrap" sheetId="2" r:id="rId2"/>
+    <sheet name="Test Case for Student breakdown" sheetId="5" r:id="rId3"/>
+    <sheet name="Test Case for Agd" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="129">
   <si>
     <t>S/N</t>
   </si>
@@ -395,16 +397,75 @@
   </si>
   <si>
     <t xml:space="preserve">Redirect to Admin DashBoard, database empty, error msgs for all rows </t>
+  </si>
+  <si>
+    <t>User: Correct time, Correct date</t>
+  </si>
+  <si>
+    <t>User: Wrong time, Correct date</t>
+  </si>
+  <si>
+    <t>User: Correct time, Wrong date</t>
+  </si>
+  <si>
+    <t>time: 10:00:02 AM
+date: 06-02-2017</t>
+  </si>
+  <si>
+    <t>time: 10:00 AM
+date: 06-02-2018</t>
+  </si>
+  <si>
+    <t>time: 10:00:02 AM
+date: 2019-02-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter time into time field and enter date under date field </t>
+  </si>
+  <si>
+    <t>User able to view four different basic location reports</t>
+  </si>
+  <si>
+    <t>User unable to view four different basic location reports</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -526,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -576,6 +637,40 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -893,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L3" sqref="A1:L3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1606,665 +1701,667 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19A71C0E-D987-4F72-8E55-1A15A93E3B4A}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="25.1796875" customWidth="1"/>
-    <col min="3" max="3" width="28.54296875" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="23"/>
+    <col min="2" max="2" width="25.1796875" style="23" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" style="23" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="10.1796875" style="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="15"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="1" t="s">
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="20" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
+      <c r="A3" s="26">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
     </row>
     <row r="4" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
+      <c r="A4" s="26">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
     </row>
     <row r="5" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
+      <c r="A5" s="26">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
     </row>
     <row r="6" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
+      <c r="A6" s="26">
         <v>4</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
     </row>
     <row r="7" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
+      <c r="A7" s="26">
         <v>5</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
     </row>
     <row r="8" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
+      <c r="A8" s="26">
         <v>6</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
     </row>
     <row r="9" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
+      <c r="A9" s="26">
         <v>7</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
     </row>
     <row r="10" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
+      <c r="A10" s="26">
         <v>8</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
     </row>
     <row r="11" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
+      <c r="A11" s="26">
         <v>9</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
     </row>
     <row r="12" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
+      <c r="A12" s="26">
         <v>10</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
     </row>
     <row r="13" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
+      <c r="A13" s="26">
         <v>11</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F13" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
     </row>
     <row r="14" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="3">
+      <c r="A14" s="26">
         <v>12</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="3">
+      <c r="A15" s="26">
         <v>13</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="3">
+      <c r="A16" s="26">
         <v>14</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="3">
+      <c r="A17" s="26">
         <v>15</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
+      <c r="A18" s="26">
         <v>16</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="3">
+      <c r="A19" s="26">
         <v>17</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="3">
+      <c r="A20" s="26">
         <v>18</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="3">
+      <c r="A21" s="26">
         <v>19</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="3">
+      <c r="A22" s="26">
         <v>20</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="3">
+      <c r="A23" s="26">
         <v>21</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="3">
+      <c r="A24" s="26">
         <v>22</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="3">
+      <c r="A25" s="26">
         <v>23</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="3">
+      <c r="A26" s="26">
         <v>24</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" s="3">
+      <c r="A27" s="26">
         <v>25</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="3">
+      <c r="A28" s="26">
         <v>26</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="3">
+      <c r="A29" s="26">
         <v>27</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="3">
+      <c r="A30" s="26">
         <v>28</v>
       </c>
-      <c r="B30" s="11"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" s="3">
+      <c r="A31" s="26">
         <v>29</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="3">
+      <c r="A32" s="26">
         <v>30</v>
       </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2279,4 +2376,582 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E40AF5E-F2E2-48FF-97C9-372CD64636EE}">
+  <dimension ref="A1:K32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="23"/>
+    <col min="2" max="2" width="28.1796875" style="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" style="23" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="10.1796875" style="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="26">
+        <v>1</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+    </row>
+    <row r="4" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="26">
+        <v>2</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+    </row>
+    <row r="5" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="26">
+        <v>3</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="26">
+        <v>4</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="26">
+        <v>5</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="26">
+        <v>6</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="26">
+        <v>7</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="26">
+        <v>8</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="26">
+        <v>9</v>
+      </c>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="26">
+        <v>10</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="26">
+        <v>11</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="26">
+        <v>12</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="26">
+        <v>13</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="26">
+        <v>14</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="26">
+        <v>15</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="26">
+        <v>16</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" s="26">
+        <v>17</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="26">
+        <v>18</v>
+      </c>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" s="26">
+        <v>19</v>
+      </c>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" s="26">
+        <v>20</v>
+      </c>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" s="26">
+        <v>21</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" s="26">
+        <v>22</v>
+      </c>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="27"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" s="26">
+        <v>23</v>
+      </c>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="28"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" s="26">
+        <v>24</v>
+      </c>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27" s="26">
+        <v>25</v>
+      </c>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28" s="26">
+        <v>26</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29" s="26">
+        <v>27</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" s="26">
+        <v>28</v>
+      </c>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31" s="26">
+        <v>29</v>
+      </c>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32" s="26">
+        <v>30</v>
+      </c>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F2175C8-B229-4B5A-99F1-6F80F2416620}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add in test cases for AGD
</commit_message>
<xml_diff>
--- a/testing/Testcases-iteration.xlsx
+++ b/testing/Testcases-iteration.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" tabRatio="1000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" tabRatio="1000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case for Login Validation" sheetId="1" r:id="rId1"/>
     <sheet name="Test Case for Bootstrap" sheetId="2" r:id="rId2"/>
     <sheet name="Test Case for Student breakdown" sheetId="5" r:id="rId3"/>
-    <sheet name="Test Case for Agd" sheetId="4" r:id="rId4"/>
+    <sheet name="Test Case for AGD" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="137">
   <si>
     <t>S/N</t>
   </si>
@@ -427,13 +427,37 @@
   </si>
   <si>
     <t>User unable to view four different basic location reports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user: Invalid day, valid hour </t>
+  </si>
+  <si>
+    <t>user: Valid day, invalid hour</t>
+  </si>
+  <si>
+    <t>user: Valid day, valid hour</t>
+  </si>
+  <si>
+    <t>date in YYYY-MM-DD format and hour in HH:MM:SS format</t>
+  </si>
+  <si>
+    <t>day in YYYY-MM-DD format, hour in MM:HH:SS format</t>
+  </si>
+  <si>
+    <t>day in DD-MM-YYYY format, hour in HH:MM:SS format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter date </t>
+  </si>
+  <si>
+    <t>Response, members, locations should be sorted according to requirements. Total time should be in seconds</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,6 +519,42 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -587,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -617,8 +677,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -638,39 +711,75 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1005,42 +1114,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="19" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="15"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="15"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="20"/>
       <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1707,661 +1816,661 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="23"/>
-    <col min="2" max="2" width="25.1796875" style="23" customWidth="1"/>
-    <col min="3" max="3" width="28.54296875" style="23" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" style="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="10.1796875" style="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="23"/>
+    <col min="1" max="1" width="8.7265625" style="12"/>
+    <col min="2" max="2" width="25.1796875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" style="12" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="10.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="20" t="s">
+      <c r="A2" s="26"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="11" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A3" s="26">
+      <c r="A3" s="13">
         <v>1</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A4" s="26">
+      <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A5" s="26">
+      <c r="A5" s="13">
         <v>3</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
     </row>
     <row r="6" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A6" s="26">
+      <c r="A6" s="13">
         <v>4</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="E6" s="27" t="s">
+      <c r="E6" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="G6" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
     </row>
     <row r="7" spans="1:11" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="26">
+      <c r="A7" s="13">
         <v>5</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
     </row>
     <row r="8" spans="1:11" ht="87" x14ac:dyDescent="0.35">
-      <c r="A8" s="26">
+      <c r="A8" s="13">
         <v>6</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
     </row>
     <row r="9" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="26">
+      <c r="A9" s="13">
         <v>7</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D9" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
     </row>
     <row r="10" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="26">
+      <c r="A10" s="13">
         <v>8</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="E10" s="27" t="s">
+      <c r="E10" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="G10" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
     </row>
     <row r="11" spans="1:11" ht="145" x14ac:dyDescent="0.35">
-      <c r="A11" s="26">
+      <c r="A11" s="13">
         <v>9</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="E11" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
     </row>
     <row r="12" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="26">
+      <c r="A12" s="13">
         <v>10</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G12" s="28" t="s">
+      <c r="G12" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
     </row>
     <row r="13" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="26">
+      <c r="A13" s="13">
         <v>11</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="D13" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="E13" s="27" t="s">
+      <c r="E13" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="F13" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="G13" s="29" t="s">
+      <c r="G13" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
     </row>
     <row r="14" spans="1:11" ht="159.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="26">
+      <c r="A14" s="13">
         <v>12</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="27" t="s">
+      <c r="F14" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G14" s="28" t="s">
+      <c r="G14" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="26">
+      <c r="A15" s="13">
         <v>13</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="26">
+      <c r="A16" s="13">
         <v>14</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="26">
+      <c r="A17" s="13">
         <v>15</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="26">
+      <c r="A18" s="13">
         <v>16</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="26">
+      <c r="A19" s="13">
         <v>17</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="26">
+      <c r="A20" s="13">
         <v>18</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="26">
+      <c r="A21" s="13">
         <v>19</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="26">
+      <c r="A22" s="13">
         <v>20</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="26">
+      <c r="A23" s="13">
         <v>21</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="26">
+      <c r="A24" s="13">
         <v>22</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="26">
+      <c r="A25" s="13">
         <v>23</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="26">
+      <c r="A26" s="13">
         <v>24</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" s="26">
+      <c r="A27" s="13">
         <v>25</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="26">
+      <c r="A28" s="13">
         <v>26</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="26">
+      <c r="A29" s="13">
         <v>27</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="26">
+      <c r="A30" s="13">
         <v>28</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" s="26">
+      <c r="A31" s="13">
         <v>29</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="28"/>
-      <c r="K31" s="28"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="26">
+      <c r="A32" s="13">
         <v>30</v>
       </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2382,552 +2491,552 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E40AF5E-F2E2-48FF-97C9-372CD64636EE}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="23"/>
-    <col min="2" max="2" width="28.1796875" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.54296875" style="23" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.1796875" style="23" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.54296875" style="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="10.1796875" style="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="23"/>
+    <col min="1" max="1" width="8.7265625" style="34"/>
+    <col min="2" max="2" width="28.1796875" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" style="34" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="10.1796875" style="34" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="20" t="s">
+      <c r="A2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="20" t="s">
+      <c r="K2" s="31" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="26">
+      <c r="A3" s="37">
         <v>1</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
     </row>
     <row r="4" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="26">
+      <c r="A4" s="37">
         <v>2</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
     </row>
     <row r="5" spans="1:11" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="26">
+      <c r="A5" s="37">
         <v>3</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="41" t="s">
         <v>122</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="46" t="s">
         <v>125</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="46" t="s">
         <v>126</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="26">
+      <c r="A6" s="37">
         <v>4</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="26">
+      <c r="A7" s="37">
         <v>5</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="26">
+      <c r="A8" s="37">
         <v>6</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="26">
+      <c r="A9" s="37">
         <v>7</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="26">
+      <c r="A10" s="37">
         <v>8</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="26">
+      <c r="A11" s="37">
         <v>9</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="26">
+      <c r="A12" s="37">
         <v>10</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="26">
+      <c r="A13" s="37">
         <v>11</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="26">
+      <c r="A14" s="37">
         <v>12</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="26">
+      <c r="A15" s="37">
         <v>13</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="39"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="26">
+      <c r="A16" s="37">
         <v>14</v>
       </c>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="28"/>
-      <c r="J16" s="28"/>
-      <c r="K16" s="28"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="26">
+      <c r="A17" s="37">
         <v>15</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="26">
+      <c r="A18" s="37">
         <v>16</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="26">
+      <c r="A19" s="37">
         <v>17</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="26">
+      <c r="A20" s="37">
         <v>18</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="26">
+      <c r="A21" s="37">
         <v>19</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="26">
+      <c r="A22" s="37">
         <v>20</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="28"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="26">
+      <c r="A23" s="37">
         <v>21</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="26">
+      <c r="A24" s="37">
         <v>22</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="26">
+      <c r="A25" s="37">
         <v>23</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="28"/>
-      <c r="K25" s="28"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="39"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="26">
+      <c r="A26" s="37">
         <v>24</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-      <c r="K26" s="28"/>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="39"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" s="26">
+      <c r="A27" s="37">
         <v>25</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-      <c r="K27" s="28"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="39"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="26">
+      <c r="A28" s="37">
         <v>26</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="26">
+      <c r="A29" s="37">
         <v>27</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="26">
+      <c r="A30" s="37">
         <v>28</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="28"/>
-      <c r="K30" s="28"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" s="26">
+      <c r="A31" s="37">
         <v>29</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="28"/>
-      <c r="K31" s="28"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="26">
+      <c r="A32" s="37">
         <v>30</v>
       </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="27"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28"/>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2945,13 +3054,561 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F2175C8-B229-4B5A-99F1-6F80F2416620}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F34C6A-AD13-489E-B8D1-D0228FED8348}">
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="34"/>
+    <col min="2" max="2" width="28.1796875" style="34" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.54296875" style="34" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" style="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1796875" style="34" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" style="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="11" width="10.1796875" style="34" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="34"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="35"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="31" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A3" s="37">
+        <v>1</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="F3" s="38"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+    </row>
+    <row r="4" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A4" s="37">
+        <v>2</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="E4" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="F4" s="38"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+    </row>
+    <row r="5" spans="1:11" ht="116" x14ac:dyDescent="0.35">
+      <c r="A5" s="37">
+        <v>3</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" s="38"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="37">
+        <v>4</v>
+      </c>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="37">
+        <v>5</v>
+      </c>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="37">
+        <v>6</v>
+      </c>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="39"/>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39"/>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="37">
+        <v>7</v>
+      </c>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="37">
+        <v>8</v>
+      </c>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="37">
+        <v>9</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
+      <c r="J11" s="39"/>
+      <c r="K11" s="39"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="37">
+        <v>10</v>
+      </c>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="39"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="37">
+        <v>11</v>
+      </c>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="37">
+        <v>12</v>
+      </c>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="37">
+        <v>13</v>
+      </c>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="39"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="37">
+        <v>14</v>
+      </c>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="37">
+        <v>15</v>
+      </c>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="37">
+        <v>16</v>
+      </c>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" s="37">
+        <v>17</v>
+      </c>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="37">
+        <v>18</v>
+      </c>
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="39"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
+      <c r="K20" s="39"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" s="37">
+        <v>19</v>
+      </c>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="39"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" s="37">
+        <v>20</v>
+      </c>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" s="37">
+        <v>21</v>
+      </c>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" s="37">
+        <v>22</v>
+      </c>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" s="37">
+        <v>23</v>
+      </c>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="39"/>
+      <c r="K25" s="39"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" s="37">
+        <v>24</v>
+      </c>
+      <c r="B26" s="38"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="39"/>
+      <c r="K26" s="39"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27" s="37">
+        <v>25</v>
+      </c>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="39"/>
+      <c r="K27" s="39"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28" s="37">
+        <v>26</v>
+      </c>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29" s="37">
+        <v>27</v>
+      </c>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" s="37">
+        <v>28</v>
+      </c>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31" s="37">
+        <v>29</v>
+      </c>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32" s="37">
+        <v>30</v>
+      </c>
+      <c r="B32" s="38"/>
+      <c r="C32" s="38"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added missed out updates on Test-case
</commit_message>
<xml_diff>
--- a/testing/Testcases-iteration.xlsx
+++ b/testing/Testcases-iteration.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" tabRatio="1000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" tabRatio="1000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case for Login Validation" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="169">
   <si>
     <t>S/N</t>
   </si>
@@ -577,12 +577,15 @@
   <si>
     <t>Error message for invalid date/time</t>
   </si>
+  <si>
+    <t>pass</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -671,13 +674,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -716,6 +712,35 @@
     <font>
       <sz val="11"/>
       <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -808,7 +833,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -861,6 +886,67 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -897,6 +983,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -909,114 +1001,50 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1352,42 +1380,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="43" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B2" s="23"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="23"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="44"/>
       <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
@@ -2066,41 +2094,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="49" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B2" s="29"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="29"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="11" t="s">
         <v>16</v>
       </c>
@@ -2730,8 +2758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E40AF5E-F2E2-48FF-97C9-372CD64636EE}">
   <dimension ref="B1:L32"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2741,61 +2769,61 @@
     <col min="3" max="3" width="28.1796875" style="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.54296875" style="17" customWidth="1"/>
     <col min="5" max="5" width="25.81640625" style="17" customWidth="1"/>
-    <col min="6" max="6" width="21.453125" style="62" customWidth="1"/>
-    <col min="7" max="7" width="20.08984375" style="62" customWidth="1"/>
-    <col min="8" max="12" width="10.1796875" style="62" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.453125" style="37" customWidth="1"/>
+    <col min="7" max="7" width="20.08984375" style="37" customWidth="1"/>
+    <col min="8" max="12" width="10.1796875" style="37" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="8.7265625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="56" t="s">
+      <c r="H1" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="I1" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B2" s="33"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="56" t="s">
+      <c r="B2" s="56"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="56" t="s">
+      <c r="I2" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="56" t="s">
+      <c r="J2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="56" t="s">
+      <c r="K2" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="56" t="s">
+      <c r="L2" s="34" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2803,270 +2831,320 @@
       <c r="B3" s="18">
         <v>1</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="G3" s="54"/>
-      <c r="H3" s="65" t="s">
+      <c r="G3" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="I3" s="59"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
+      <c r="I3" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
     </row>
     <row r="4" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B4" s="18">
         <v>2</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="F4" s="64" t="s">
+      <c r="F4" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="G4" s="64"/>
-      <c r="H4" s="65" t="s">
+      <c r="G4" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
+      <c r="I4" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
     </row>
     <row r="5" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B5" s="18">
         <v>3</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="32" t="s">
         <v>130</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="F5" s="64" t="s">
+      <c r="F5" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="G5" s="64"/>
-      <c r="H5" s="65" t="s">
+      <c r="G5" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="H5" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
+      <c r="I5" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
     </row>
     <row r="6" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B6" s="18">
         <v>4</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="D6" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="E6" s="54" t="s">
+      <c r="E6" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="F6" s="64" t="s">
+      <c r="F6" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="G6" s="64"/>
-      <c r="H6" s="65" t="s">
+      <c r="G6" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
+      <c r="I6" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
     </row>
     <row r="7" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B7" s="18">
         <v>5</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="38" t="s">
         <v>142</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="E7" s="54" t="s">
+      <c r="E7" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="F7" s="64" t="s">
+      <c r="F7" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="G7" s="64"/>
-      <c r="H7" s="65" t="s">
+      <c r="G7" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="H7" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
+      <c r="I7" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
     </row>
     <row r="8" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B8" s="18">
         <v>6</v>
       </c>
-      <c r="C8" s="63" t="s">
+      <c r="C8" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="E8" s="54" t="s">
+      <c r="E8" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="F8" s="64" t="s">
+      <c r="F8" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="G8" s="64"/>
-      <c r="H8" s="65" t="s">
+      <c r="G8" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="H8" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
+      <c r="I8" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
     </row>
     <row r="9" spans="2:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B9" s="18">
         <v>7</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="D9" s="63" t="s">
+      <c r="D9" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="54" t="s">
+      <c r="E9" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="F9" s="64" t="s">
+      <c r="F9" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="G9" s="64"/>
-      <c r="H9" s="65" t="s">
+      <c r="G9" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="H9" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
+      <c r="I9" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
     </row>
     <row r="10" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B10" s="18">
         <v>8</v>
       </c>
-      <c r="C10" s="54" t="s">
+      <c r="C10" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="38" t="s">
         <v>151</v>
       </c>
-      <c r="E10" s="54" t="s">
+      <c r="E10" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="F10" s="64" t="s">
+      <c r="F10" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="G10" s="19"/>
-      <c r="H10" s="65" t="s">
+      <c r="G10" s="39" t="s">
+        <v>134</v>
+      </c>
+      <c r="H10" s="40" t="s">
         <v>146</v>
       </c>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="60"/>
-      <c r="L10" s="60"/>
+      <c r="I10" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
     </row>
     <row r="11" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B11" s="18">
         <v>9</v>
       </c>
-      <c r="C11" s="63" t="s">
+      <c r="C11" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="D11" s="63" t="s">
+      <c r="D11" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="E11" s="54" t="s">
+      <c r="E11" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="F11" s="64" t="s">
+      <c r="F11" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="G11" s="19"/>
-      <c r="H11" s="60"/>
-      <c r="I11" s="60"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="60"/>
-      <c r="L11" s="60"/>
+      <c r="G11" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="H11" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="I11" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
     </row>
     <row r="12" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B12" s="18">
         <v>10</v>
       </c>
-      <c r="C12" s="63" t="s">
+      <c r="C12" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="D12" s="63" t="s">
+      <c r="D12" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="E12" s="54" t="s">
+      <c r="E12" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="F12" s="64" t="s">
+      <c r="F12" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="G12" s="19"/>
-      <c r="H12" s="60"/>
-      <c r="I12" s="60"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="60"/>
-      <c r="L12" s="60"/>
+      <c r="G12" s="39" t="s">
+        <v>136</v>
+      </c>
+      <c r="H12" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="I12" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
     </row>
     <row r="13" spans="2:12" ht="87" x14ac:dyDescent="0.35">
       <c r="B13" s="18">
         <v>11</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="C13" s="38" t="s">
         <v>147</v>
       </c>
-      <c r="D13" s="63" t="s">
+      <c r="D13" s="38" t="s">
         <v>151</v>
       </c>
-      <c r="E13" s="54" t="s">
+      <c r="E13" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="F13" s="64" t="s">
+      <c r="F13" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="G13" s="64"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="60"/>
+      <c r="G13" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="H13" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="I13" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B14" s="18">
@@ -3077,11 +3155,11 @@
       <c r="E14" s="19"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-      <c r="L14" s="60"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B15" s="18">
@@ -3092,11 +3170,11 @@
       <c r="E15" s="19"/>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="60"/>
-      <c r="L15" s="60"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+      <c r="K15" s="36"/>
+      <c r="L15" s="36"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="18">
@@ -3107,11 +3185,11 @@
       <c r="E16" s="19"/>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
-      <c r="H16" s="60"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="60"/>
-      <c r="L16" s="60"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B17" s="18">
@@ -3122,11 +3200,11 @@
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="60"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="60"/>
-      <c r="L17" s="60"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18" s="18">
@@ -3137,11 +3215,11 @@
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
-      <c r="H18" s="60"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="60"/>
-      <c r="L18" s="60"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B19" s="18">
@@ -3152,11 +3230,11 @@
       <c r="E19" s="19"/>
       <c r="F19" s="19"/>
       <c r="G19" s="19"/>
-      <c r="H19" s="60"/>
-      <c r="I19" s="60"/>
-      <c r="J19" s="60"/>
-      <c r="K19" s="60"/>
-      <c r="L19" s="60"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B20" s="18">
@@ -3167,11 +3245,11 @@
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
-      <c r="H20" s="60"/>
-      <c r="I20" s="60"/>
-      <c r="J20" s="60"/>
-      <c r="K20" s="60"/>
-      <c r="L20" s="60"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B21" s="18">
@@ -3182,11 +3260,11 @@
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
-      <c r="H21" s="60"/>
-      <c r="I21" s="60"/>
-      <c r="J21" s="60"/>
-      <c r="K21" s="60"/>
-      <c r="L21" s="60"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B22" s="18">
@@ -3197,11 +3275,11 @@
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
-      <c r="H22" s="60"/>
-      <c r="I22" s="60"/>
-      <c r="J22" s="60"/>
-      <c r="K22" s="60"/>
-      <c r="L22" s="60"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B23" s="18">
@@ -3212,11 +3290,11 @@
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
       <c r="G23" s="19"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="60"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B24" s="18">
@@ -3227,11 +3305,11 @@
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
-      <c r="H24" s="60"/>
-      <c r="I24" s="60"/>
-      <c r="J24" s="60"/>
-      <c r="K24" s="60"/>
-      <c r="L24" s="60"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B25" s="18">
@@ -3242,11 +3320,11 @@
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
       <c r="G25" s="19"/>
-      <c r="H25" s="60"/>
-      <c r="I25" s="60"/>
-      <c r="J25" s="60"/>
-      <c r="K25" s="60"/>
-      <c r="L25" s="60"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B26" s="18">
@@ -3257,11 +3335,11 @@
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
-      <c r="H26" s="60"/>
-      <c r="I26" s="60"/>
-      <c r="J26" s="60"/>
-      <c r="K26" s="60"/>
-      <c r="L26" s="60"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B27" s="18">
@@ -3272,11 +3350,11 @@
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
-      <c r="H27" s="60"/>
-      <c r="I27" s="60"/>
-      <c r="J27" s="60"/>
-      <c r="K27" s="60"/>
-      <c r="L27" s="60"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B28" s="18">
@@ -3287,11 +3365,11 @@
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
       <c r="G28" s="19"/>
-      <c r="H28" s="60"/>
-      <c r="I28" s="60"/>
-      <c r="J28" s="60"/>
-      <c r="K28" s="60"/>
-      <c r="L28" s="60"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="36"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B29" s="18">
@@ -3302,11 +3380,11 @@
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
       <c r="G29" s="19"/>
-      <c r="H29" s="60"/>
-      <c r="I29" s="60"/>
-      <c r="J29" s="60"/>
-      <c r="K29" s="60"/>
-      <c r="L29" s="60"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="36"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B30" s="18">
@@ -3317,11 +3395,11 @@
       <c r="E30" s="19"/>
       <c r="F30" s="19"/>
       <c r="G30" s="19"/>
-      <c r="H30" s="60"/>
-      <c r="I30" s="60"/>
-      <c r="J30" s="60"/>
-      <c r="K30" s="60"/>
-      <c r="L30" s="60"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="36"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="36"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B31" s="18">
@@ -3332,11 +3410,11 @@
       <c r="E31" s="19"/>
       <c r="F31" s="19"/>
       <c r="G31" s="19"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="60"/>
-      <c r="J31" s="60"/>
-      <c r="K31" s="60"/>
-      <c r="L31" s="60"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="36"/>
+      <c r="J31" s="36"/>
+      <c r="K31" s="36"/>
+      <c r="L31" s="36"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B32" s="18">
@@ -3347,11 +3425,11 @@
       <c r="E32" s="19"/>
       <c r="F32" s="19"/>
       <c r="G32" s="19"/>
-      <c r="H32" s="60"/>
-      <c r="I32" s="60"/>
-      <c r="J32" s="60"/>
-      <c r="K32" s="60"/>
-      <c r="L32" s="60"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3378,541 +3456,541 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.26953125" style="41" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="41"/>
-    <col min="3" max="3" width="28.1796875" style="41" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.54296875" style="41" customWidth="1"/>
-    <col min="5" max="5" width="18.26953125" style="41" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.1796875" style="41" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" style="41" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="10.1796875" style="41" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7265625" style="41"/>
+    <col min="1" max="1" width="3.26953125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="21"/>
+    <col min="3" max="3" width="28.1796875" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.54296875" style="21" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" style="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="10.1796875" style="21" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B2" s="42"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="38" t="s">
+      <c r="B2" s="62"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="38" t="s">
+      <c r="I2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="38" t="s">
+      <c r="J2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="K2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="38" t="s">
+      <c r="L2" s="20" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="116" x14ac:dyDescent="0.35">
-      <c r="B3" s="44">
+      <c r="B3" s="22">
         <v>1</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="48"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="49"/>
-      <c r="L3" s="49"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
     </row>
     <row r="4" spans="2:12" ht="116" x14ac:dyDescent="0.35">
-      <c r="B4" s="44">
+      <c r="B4" s="22">
         <v>2</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="E4" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="F4" s="47" t="s">
+      <c r="F4" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="G4" s="48"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="49"/>
-      <c r="J4" s="49"/>
-      <c r="K4" s="49"/>
-      <c r="L4" s="49"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
     </row>
     <row r="5" spans="2:12" ht="116" x14ac:dyDescent="0.35">
-      <c r="B5" s="44">
+      <c r="B5" s="22">
         <v>3</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="G5" s="48"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B6" s="44">
+      <c r="B6" s="22">
         <v>4</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B7" s="44">
+      <c r="B7" s="22">
         <v>5</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="49"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="44">
+      <c r="B8" s="22">
         <v>6</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B9" s="44">
+      <c r="B9" s="22">
         <v>7</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
-      <c r="K9" s="49"/>
-      <c r="L9" s="49"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B10" s="44">
+      <c r="B10" s="22">
         <v>8</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
-      <c r="J10" s="49"/>
-      <c r="K10" s="49"/>
-      <c r="L10" s="49"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B11" s="44">
+      <c r="B11" s="22">
         <v>9</v>
       </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="49"/>
-      <c r="I11" s="49"/>
-      <c r="J11" s="49"/>
-      <c r="K11" s="49"/>
-      <c r="L11" s="49"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
+      <c r="L11" s="27"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B12" s="44">
+      <c r="B12" s="22">
         <v>10</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="49"/>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="49"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B13" s="44">
+      <c r="B13" s="22">
         <v>11</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="49"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B14" s="44">
+      <c r="B14" s="22">
         <v>12</v>
       </c>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="49"/>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="49"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B15" s="44">
+      <c r="B15" s="22">
         <v>13</v>
       </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="49"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B16" s="44">
+      <c r="B16" s="22">
         <v>14</v>
       </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="49"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B17" s="44">
+      <c r="B17" s="22">
         <v>15</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="49"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B18" s="44">
+      <c r="B18" s="22">
         <v>16</v>
       </c>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
-      <c r="K18" s="49"/>
-      <c r="L18" s="49"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B19" s="44">
+      <c r="B19" s="22">
         <v>17</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="49"/>
-      <c r="L19" s="49"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B20" s="44">
+      <c r="B20" s="22">
         <v>18</v>
       </c>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="49"/>
-      <c r="L20" s="49"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B21" s="44">
+      <c r="B21" s="22">
         <v>19</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="49"/>
-      <c r="K21" s="49"/>
-      <c r="L21" s="49"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B22" s="44">
+      <c r="B22" s="22">
         <v>20</v>
       </c>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B23" s="44">
+      <c r="B23" s="22">
         <v>21</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="49"/>
-      <c r="J23" s="49"/>
-      <c r="K23" s="49"/>
-      <c r="L23" s="49"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B24" s="44">
+      <c r="B24" s="22">
         <v>22</v>
       </c>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="49"/>
-      <c r="L24" s="49"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="27"/>
+      <c r="I24" s="27"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B25" s="44">
+      <c r="B25" s="22">
         <v>23</v>
       </c>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="49"/>
-      <c r="J25" s="49"/>
-      <c r="K25" s="49"/>
-      <c r="L25" s="49"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B26" s="44">
+      <c r="B26" s="22">
         <v>24</v>
       </c>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="49"/>
-      <c r="J26" s="49"/>
-      <c r="K26" s="49"/>
-      <c r="L26" s="49"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B27" s="44">
+      <c r="B27" s="22">
         <v>25</v>
       </c>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="49"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="49"/>
-      <c r="K27" s="49"/>
-      <c r="L27" s="49"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="27"/>
+      <c r="I27" s="27"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="27"/>
+      <c r="L27" s="27"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B28" s="44">
+      <c r="B28" s="22">
         <v>26</v>
       </c>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
-      <c r="K28" s="49"/>
-      <c r="L28" s="49"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="27"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B29" s="44">
+      <c r="B29" s="22">
         <v>27</v>
       </c>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="48"/>
-      <c r="H29" s="49"/>
-      <c r="I29" s="49"/>
-      <c r="J29" s="49"/>
-      <c r="K29" s="49"/>
-      <c r="L29" s="49"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B30" s="44">
+      <c r="B30" s="22">
         <v>28</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="49"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="49"/>
-      <c r="K30" s="49"/>
-      <c r="L30" s="49"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="27"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B31" s="44">
+      <c r="B31" s="22">
         <v>29</v>
       </c>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="49"/>
-      <c r="I31" s="49"/>
-      <c r="J31" s="49"/>
-      <c r="K31" s="49"/>
-      <c r="L31" s="49"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="27"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B32" s="44">
+      <c r="B32" s="22">
         <v>30</v>
       </c>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="49"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="49"/>
-      <c r="K32" s="49"/>
-      <c r="L32" s="49"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
+      <c r="J32" s="27"/>
+      <c r="K32" s="27"/>
+      <c r="L32" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3933,72 +4011,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51635F72-9BA6-4F0C-99B9-3FC01EDB15BB}">
   <dimension ref="B1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.26953125" style="66" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625" style="66"/>
-    <col min="3" max="3" width="28.1796875" style="66" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.54296875" style="66" customWidth="1"/>
-    <col min="5" max="5" width="18.26953125" style="66" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.81640625" style="66" customWidth="1"/>
-    <col min="7" max="7" width="24.08984375" style="66" customWidth="1"/>
-    <col min="8" max="12" width="10.1796875" style="66" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7265625" style="66"/>
+    <col min="1" max="1" width="3.26953125" style="67" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="67"/>
+    <col min="3" max="3" width="28.1796875" style="67" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.54296875" style="67" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" style="67" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.81640625" style="67" customWidth="1"/>
+    <col min="7" max="7" width="24.08984375" style="67" customWidth="1"/>
+    <col min="8" max="12" width="10.1796875" style="67" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="67"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="71" t="s">
+      <c r="D1" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="71" t="s">
+      <c r="F1" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="71" t="s">
+      <c r="G1" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="67" t="s">
+      <c r="H1" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="71" t="s">
+      <c r="I1" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="67" t="s">
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="67" t="s">
+      <c r="I2" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="67" t="s">
+      <c r="J2" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="67" t="s">
+      <c r="K2" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="67" t="s">
+      <c r="L2" s="66" t="s">
         <v>48</v>
       </c>
     </row>
@@ -4006,475 +4084,475 @@
       <c r="B3" s="68">
         <v>1</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="69" t="s">
         <v>159</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="69" t="s">
         <v>157</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="69" t="s">
         <v>158</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="69" t="s">
         <v>166</v>
       </c>
-      <c r="G3" s="48"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
     </row>
     <row r="4" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B4" s="68">
         <v>2</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="69" t="s">
         <v>160</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="69" t="s">
         <v>162</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="E4" s="69" t="s">
         <v>165</v>
       </c>
-      <c r="F4" s="47" t="s">
+      <c r="F4" s="69" t="s">
         <v>167</v>
       </c>
-      <c r="G4" s="48"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="71"/>
     </row>
     <row r="5" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B5" s="68">
         <v>3</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="69" t="s">
         <v>161</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="69" t="s">
         <v>163</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="69" t="s">
         <v>164</v>
       </c>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="69" t="s">
         <v>167</v>
       </c>
-      <c r="G5" s="48"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="71"/>
+      <c r="L5" s="71"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="68">
         <v>4</v>
       </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="69"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
+      <c r="L6" s="71"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B7" s="68">
         <v>5</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
-      <c r="G7" s="48"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="71"/>
+      <c r="L7" s="71"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B8" s="68">
         <v>6</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="71"/>
+      <c r="K8" s="71"/>
+      <c r="L8" s="71"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B9" s="68">
         <v>7</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="69"/>
-      <c r="K9" s="69"/>
-      <c r="L9" s="69"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="71"/>
+      <c r="L9" s="71"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10" s="68">
         <v>8</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="69"/>
-      <c r="L10" s="69"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="71"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11" s="68">
         <v>9</v>
       </c>
       <c r="C11" s="72"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="69"/>
-      <c r="L11" s="69"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="71"/>
+      <c r="J11" s="71"/>
+      <c r="K11" s="71"/>
+      <c r="L11" s="71"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B12" s="68">
         <v>10</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="48"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
-      <c r="G12" s="48"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="71"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="71"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B13" s="68">
         <v>11</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="48"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
-      <c r="G13" s="48"/>
-      <c r="H13" s="70"/>
-      <c r="I13" s="69"/>
-      <c r="J13" s="69"/>
-      <c r="K13" s="69"/>
-      <c r="L13" s="69"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="70"/>
+      <c r="E13" s="70"/>
+      <c r="F13" s="70"/>
+      <c r="G13" s="70"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="71"/>
+      <c r="J13" s="71"/>
+      <c r="K13" s="71"/>
+      <c r="L13" s="71"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B14" s="68">
         <v>12</v>
       </c>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="69"/>
-      <c r="I14" s="69"/>
-      <c r="J14" s="69"/>
-      <c r="K14" s="69"/>
-      <c r="L14" s="69"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="70"/>
+      <c r="E14" s="70"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="70"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="71"/>
+      <c r="K14" s="71"/>
+      <c r="L14" s="71"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B15" s="68">
         <v>13</v>
       </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="69"/>
-      <c r="J15" s="69"/>
-      <c r="K15" s="69"/>
-      <c r="L15" s="69"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="70"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="70"/>
+      <c r="G15" s="70"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="71"/>
+      <c r="J15" s="71"/>
+      <c r="K15" s="71"/>
+      <c r="L15" s="71"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="68">
         <v>14</v>
       </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="69"/>
-      <c r="I16" s="69"/>
-      <c r="J16" s="69"/>
-      <c r="K16" s="69"/>
-      <c r="L16" s="69"/>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70"/>
+      <c r="E16" s="70"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="70"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="71"/>
+      <c r="L16" s="71"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B17" s="68">
         <v>15</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="69"/>
-      <c r="I17" s="69"/>
-      <c r="J17" s="69"/>
-      <c r="K17" s="69"/>
-      <c r="L17" s="69"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="71"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18" s="68">
         <v>16</v>
       </c>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="69"/>
-      <c r="I18" s="69"/>
-      <c r="J18" s="69"/>
-      <c r="K18" s="69"/>
-      <c r="L18" s="69"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
+      <c r="K18" s="71"/>
+      <c r="L18" s="71"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B19" s="68">
         <v>17</v>
       </c>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="69"/>
-      <c r="I19" s="69"/>
-      <c r="J19" s="69"/>
-      <c r="K19" s="69"/>
-      <c r="L19" s="69"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="71"/>
+      <c r="J19" s="71"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="71"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B20" s="68">
         <v>18</v>
       </c>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="69"/>
-      <c r="I20" s="69"/>
-      <c r="J20" s="69"/>
-      <c r="K20" s="69"/>
-      <c r="L20" s="69"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="71"/>
+      <c r="J20" s="71"/>
+      <c r="K20" s="71"/>
+      <c r="L20" s="71"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B21" s="68">
         <v>19</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="69"/>
-      <c r="I21" s="69"/>
-      <c r="J21" s="69"/>
-      <c r="K21" s="69"/>
-      <c r="L21" s="69"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="70"/>
+      <c r="E21" s="70"/>
+      <c r="F21" s="70"/>
+      <c r="G21" s="70"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="71"/>
+      <c r="K21" s="71"/>
+      <c r="L21" s="71"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B22" s="68">
         <v>20</v>
       </c>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="69"/>
-      <c r="I22" s="69"/>
-      <c r="J22" s="69"/>
-      <c r="K22" s="69"/>
-      <c r="L22" s="69"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="71"/>
+      <c r="J22" s="71"/>
+      <c r="K22" s="71"/>
+      <c r="L22" s="71"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B23" s="68">
         <v>21</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
-      <c r="H23" s="69"/>
-      <c r="I23" s="69"/>
-      <c r="J23" s="69"/>
-      <c r="K23" s="69"/>
-      <c r="L23" s="69"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="70"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="70"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="71"/>
+      <c r="K23" s="71"/>
+      <c r="L23" s="71"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B24" s="68">
         <v>22</v>
       </c>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="69"/>
-      <c r="I24" s="69"/>
-      <c r="J24" s="69"/>
-      <c r="K24" s="69"/>
-      <c r="L24" s="69"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="71"/>
+      <c r="K24" s="71"/>
+      <c r="L24" s="71"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B25" s="68">
         <v>23</v>
       </c>
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="69"/>
-      <c r="I25" s="69"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="69"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="70"/>
+      <c r="F25" s="70"/>
+      <c r="G25" s="70"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="71"/>
+      <c r="J25" s="71"/>
+      <c r="K25" s="71"/>
+      <c r="L25" s="71"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B26" s="68">
         <v>24</v>
       </c>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="69"/>
-      <c r="I26" s="69"/>
-      <c r="J26" s="69"/>
-      <c r="K26" s="69"/>
-      <c r="L26" s="69"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="70"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="70"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="71"/>
+      <c r="J26" s="71"/>
+      <c r="K26" s="71"/>
+      <c r="L26" s="71"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B27" s="68">
         <v>25</v>
       </c>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="48"/>
-      <c r="H27" s="69"/>
-      <c r="I27" s="69"/>
-      <c r="J27" s="69"/>
-      <c r="K27" s="69"/>
-      <c r="L27" s="69"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="71"/>
+      <c r="I27" s="71"/>
+      <c r="J27" s="71"/>
+      <c r="K27" s="71"/>
+      <c r="L27" s="71"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B28" s="68">
         <v>26</v>
       </c>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="69"/>
-      <c r="I28" s="69"/>
-      <c r="J28" s="69"/>
-      <c r="K28" s="69"/>
-      <c r="L28" s="69"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
+      <c r="K28" s="71"/>
+      <c r="L28" s="71"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B29" s="68">
         <v>27</v>
       </c>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="48"/>
-      <c r="H29" s="69"/>
-      <c r="I29" s="69"/>
-      <c r="J29" s="69"/>
-      <c r="K29" s="69"/>
-      <c r="L29" s="69"/>
+      <c r="C29" s="70"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="70"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="70"/>
+      <c r="H29" s="71"/>
+      <c r="I29" s="71"/>
+      <c r="J29" s="71"/>
+      <c r="K29" s="71"/>
+      <c r="L29" s="71"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B30" s="68">
         <v>28</v>
       </c>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="69"/>
-      <c r="J30" s="69"/>
-      <c r="K30" s="69"/>
-      <c r="L30" s="69"/>
+      <c r="C30" s="70"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="70"/>
+      <c r="H30" s="71"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="71"/>
+      <c r="K30" s="71"/>
+      <c r="L30" s="71"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B31" s="68">
         <v>29</v>
       </c>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="69"/>
-      <c r="J31" s="69"/>
-      <c r="K31" s="69"/>
-      <c r="L31" s="69"/>
+      <c r="C31" s="70"/>
+      <c r="D31" s="70"/>
+      <c r="E31" s="70"/>
+      <c r="F31" s="70"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="71"/>
+      <c r="I31" s="71"/>
+      <c r="J31" s="71"/>
+      <c r="K31" s="71"/>
+      <c r="L31" s="71"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B32" s="68">
         <v>30</v>
       </c>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="69"/>
-      <c r="J32" s="69"/>
-      <c r="K32" s="69"/>
-      <c r="L32" s="69"/>
+      <c r="C32" s="70"/>
+      <c r="D32" s="70"/>
+      <c r="E32" s="70"/>
+      <c r="F32" s="70"/>
+      <c r="G32" s="70"/>
+      <c r="H32" s="71"/>
+      <c r="I32" s="71"/>
+      <c r="J32" s="71"/>
+      <c r="K32" s="71"/>
+      <c r="L32" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Debugging overall, Add a new ValidatorException.java for bootstrap.
Adjusted bug metrics and Testcases-iteration.xlsx
</commit_message>
<xml_diff>
--- a/testing/Testcases-iteration.xlsx
+++ b/testing/Testcases-iteration.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" tabRatio="1000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" tabRatio="1000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case for Login Validation" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="220">
   <si>
     <t>S/N</t>
   </si>
@@ -257,9 +257,6 @@
     <t>Redirect back to login page.</t>
   </si>
   <si>
-    <t>Home.jsp View</t>
-  </si>
-  <si>
     <t>Fail</t>
   </si>
   <si>
@@ -269,9 +266,6 @@
     <t>User changes web URL directory to access admin.jsp</t>
   </si>
   <si>
-    <t>Admin.jsp View</t>
-  </si>
-  <si>
     <t>Admin bootstraps a .mp4 file</t>
   </si>
   <si>
@@ -336,9 +330,6 @@
   </si>
   <si>
     <t xml:space="preserve"> this-testcase.doc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> this-mixcase.mp4</t>
   </si>
   <si>
     <t>location-lookup.zip</t>
@@ -674,6 +665,75 @@
   </si>
   <si>
     <t>user: Valid time, missing date</t>
+  </si>
+  <si>
+    <t>Admin:                  empty  name, correct password</t>
+  </si>
+  <si>
+    <t>username:      password: AdminPW</t>
+  </si>
+  <si>
+    <t>Enter correct password but leave username field blank. Then submit</t>
+  </si>
+  <si>
+    <t>Form doesn’t get passed in, message "please fill out this field " appears</t>
+  </si>
+  <si>
+    <t>Form doesn’t get passed in, page doesn’t submit</t>
+  </si>
+  <si>
+    <t>User tried to access Admin.jsp</t>
+  </si>
+  <si>
+    <t>User tried to access BreakdownReports.jsp</t>
+  </si>
+  <si>
+    <t>/BreakdownReports.jsp</t>
+  </si>
+  <si>
+    <t>User changes web URL directory to access BreakdownReports.jsp</t>
+  </si>
+  <si>
+    <t>User tried to access BasicLocationReports.jsp</t>
+  </si>
+  <si>
+    <t>/BasicLocationReports.jsp</t>
+  </si>
+  <si>
+    <t>User changes web URL directory to access BasicLocationReports.jsp</t>
+  </si>
+  <si>
+    <t>User tried to access TopkReports.jsp</t>
+  </si>
+  <si>
+    <t>/TopkReports.jsp</t>
+  </si>
+  <si>
+    <t>User changes web URL directory to access TopkReports.jsp</t>
+  </si>
+  <si>
+    <t>User tried to access HeatMaps.jsp</t>
+  </si>
+  <si>
+    <t>/HeatMaps.jsp</t>
+  </si>
+  <si>
+    <t>User changes web URL directory to access HeatMaps.jsp</t>
+  </si>
+  <si>
+    <t>User tried to access AutomaticGroupIdentification.jsp</t>
+  </si>
+  <si>
+    <t>/AutomaticGroupIdentification.jsp</t>
+  </si>
+  <si>
+    <t>User changes web URL directory to accessAutomaticGroupIdentification.jsp</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> this-mixcase.zip</t>
   </si>
 </sst>
 </file>
@@ -928,7 +988,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1026,6 +1086,37 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1080,56 +1171,28 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1446,10 +1509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:M29"/>
+  <dimension ref="B1:M36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M5" sqref="B5:M5"/>
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1466,42 +1529,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="48" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="38"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="38"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="49"/>
       <c r="H2" s="25" t="s">
         <v>10</v>
       </c>
@@ -1546,7 +1609,9 @@
       <c r="I3" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="29"/>
+      <c r="J3" s="29" t="s">
+        <v>7</v>
+      </c>
       <c r="K3" s="29"/>
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
@@ -1576,12 +1641,14 @@
       <c r="I4" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="29"/>
+      <c r="J4" s="29" t="s">
+        <v>7</v>
+      </c>
       <c r="K4" s="29"/>
       <c r="L4" s="29"/>
       <c r="M4" s="29"/>
     </row>
-    <row r="5" spans="2:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" ht="75" x14ac:dyDescent="0.25">
       <c r="B5" s="27">
         <v>3</v>
       </c>
@@ -1594,11 +1661,11 @@
       <c r="E5" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="28" t="s">
-        <v>24</v>
+      <c r="F5" s="71" t="s">
+        <v>201</v>
+      </c>
+      <c r="G5" s="71" t="s">
+        <v>200</v>
       </c>
       <c r="H5" s="29" t="s">
         <v>7</v>
@@ -1606,7 +1673,9 @@
       <c r="I5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="29"/>
+      <c r="J5" s="29" t="s">
+        <v>7</v>
+      </c>
       <c r="K5" s="29"/>
       <c r="L5" s="29"/>
       <c r="M5" s="29"/>
@@ -1636,7 +1705,9 @@
       <c r="I6" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="29"/>
+      <c r="J6" s="29" t="s">
+        <v>7</v>
+      </c>
       <c r="K6" s="29"/>
       <c r="L6" s="29"/>
       <c r="M6" s="29"/>
@@ -1666,12 +1737,14 @@
       <c r="I7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="29"/>
+      <c r="J7" s="29" t="s">
+        <v>7</v>
+      </c>
       <c r="K7" s="29"/>
       <c r="L7" s="29"/>
       <c r="M7" s="29"/>
     </row>
-    <row r="8" spans="2:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="75" x14ac:dyDescent="0.25">
       <c r="B8" s="27">
         <v>6</v>
       </c>
@@ -1684,11 +1757,11 @@
       <c r="E8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="28" t="s">
-        <v>24</v>
+      <c r="F8" s="71" t="s">
+        <v>201</v>
+      </c>
+      <c r="G8" s="71" t="s">
+        <v>200</v>
       </c>
       <c r="H8" s="29" t="s">
         <v>7</v>
@@ -1696,12 +1769,14 @@
       <c r="I8" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="29"/>
+      <c r="J8" s="29" t="s">
+        <v>7</v>
+      </c>
       <c r="K8" s="29"/>
       <c r="L8" s="29"/>
       <c r="M8" s="29"/>
     </row>
-    <row r="9" spans="2:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="75" x14ac:dyDescent="0.25">
       <c r="B9" s="27">
         <v>7</v>
       </c>
@@ -1714,11 +1789,11 @@
       <c r="E9" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="28" t="s">
-        <v>24</v>
+      <c r="F9" s="71" t="s">
+        <v>201</v>
+      </c>
+      <c r="G9" s="71" t="s">
+        <v>200</v>
       </c>
       <c r="H9" s="29" t="s">
         <v>7</v>
@@ -1726,7 +1801,9 @@
       <c r="I9" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="29"/>
+      <c r="J9" s="29" t="s">
+        <v>7</v>
+      </c>
       <c r="K9" s="29"/>
       <c r="L9" s="29"/>
       <c r="M9" s="29"/>
@@ -1756,12 +1833,14 @@
       <c r="I10" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J10" s="29"/>
+      <c r="J10" s="29" t="s">
+        <v>7</v>
+      </c>
       <c r="K10" s="29"/>
       <c r="L10" s="29"/>
       <c r="M10" s="29"/>
     </row>
-    <row r="11" spans="2:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" ht="75" x14ac:dyDescent="0.25">
       <c r="B11" s="27">
         <v>9</v>
       </c>
@@ -1774,11 +1853,11 @@
       <c r="E11" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="28" t="s">
-        <v>24</v>
+      <c r="F11" s="71" t="s">
+        <v>201</v>
+      </c>
+      <c r="G11" s="71" t="s">
+        <v>200</v>
       </c>
       <c r="H11" s="29" t="s">
         <v>7</v>
@@ -1786,36 +1865,34 @@
       <c r="I11" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J11" s="29"/>
+      <c r="J11" s="29" t="s">
+        <v>7</v>
+      </c>
       <c r="K11" s="29"/>
       <c r="L11" s="29"/>
       <c r="M11" s="29"/>
     </row>
-    <row r="12" spans="2:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" s="27">
         <v>10</v>
       </c>
-      <c r="C12" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" s="29" t="s">
-        <v>7</v>
-      </c>
+      <c r="C12" s="71" t="s">
+        <v>197</v>
+      </c>
+      <c r="D12" s="71" t="s">
+        <v>198</v>
+      </c>
+      <c r="E12" s="71" t="s">
+        <v>199</v>
+      </c>
+      <c r="F12" s="71" t="s">
+        <v>201</v>
+      </c>
+      <c r="G12" s="71" t="s">
+        <v>200</v>
+      </c>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
       <c r="J12" s="29"/>
       <c r="K12" s="29"/>
       <c r="L12" s="29"/>
@@ -1826,19 +1903,19 @@
         <v>11</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="H13" s="29" t="s">
         <v>7</v>
@@ -1846,7 +1923,9 @@
       <c r="I13" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J13" s="29"/>
+      <c r="J13" s="29" t="s">
+        <v>7</v>
+      </c>
       <c r="K13" s="29"/>
       <c r="L13" s="29"/>
       <c r="M13" s="29"/>
@@ -1856,19 +1935,19 @@
         <v>12</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E14" s="28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F14" s="28" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="G14" s="28" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="H14" s="29" t="s">
         <v>7</v>
@@ -1876,29 +1955,31 @@
       <c r="I14" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="29"/>
+      <c r="J14" s="29" t="s">
+        <v>7</v>
+      </c>
       <c r="K14" s="29"/>
       <c r="L14" s="29"/>
       <c r="M14" s="29"/>
     </row>
-    <row r="15" spans="2:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="90" x14ac:dyDescent="0.25">
       <c r="B15" s="27">
         <v>13</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="28" t="s">
-        <v>14</v>
+        <v>54</v>
+      </c>
+      <c r="F15" s="71" t="s">
+        <v>201</v>
+      </c>
+      <c r="G15" s="71" t="s">
+        <v>200</v>
       </c>
       <c r="H15" s="29" t="s">
         <v>7</v>
@@ -1906,23 +1987,25 @@
       <c r="I15" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J15" s="29"/>
+      <c r="J15" s="29" t="s">
+        <v>7</v>
+      </c>
       <c r="K15" s="29"/>
       <c r="L15" s="29"/>
       <c r="M15" s="29"/>
     </row>
     <row r="16" spans="2:13" ht="105" x14ac:dyDescent="0.25">
       <c r="B16" s="27">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F16" s="28" t="s">
         <v>14</v>
@@ -1936,29 +2019,31 @@
       <c r="I16" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J16" s="29"/>
+      <c r="J16" s="29" t="s">
+        <v>7</v>
+      </c>
       <c r="K16" s="29"/>
       <c r="L16" s="29"/>
       <c r="M16" s="29"/>
     </row>
-    <row r="17" spans="2:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" ht="75" x14ac:dyDescent="0.25">
       <c r="B17" s="27">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="F17" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="28" t="s">
-        <v>14</v>
+        <v>60</v>
+      </c>
+      <c r="F17" s="71" t="s">
+        <v>201</v>
+      </c>
+      <c r="G17" s="71" t="s">
+        <v>200</v>
       </c>
       <c r="H17" s="29" t="s">
         <v>7</v>
@@ -1966,23 +2051,25 @@
       <c r="I17" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J17" s="29"/>
+      <c r="J17" s="29" t="s">
+        <v>7</v>
+      </c>
       <c r="K17" s="29"/>
       <c r="L17" s="29"/>
       <c r="M17" s="29"/>
     </row>
     <row r="18" spans="2:13" ht="105" x14ac:dyDescent="0.25">
       <c r="B18" s="27">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="F18" s="28" t="s">
         <v>14</v>
@@ -1996,174 +2083,280 @@
       <c r="I18" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J18" s="29"/>
+      <c r="J18" s="29" t="s">
+        <v>7</v>
+      </c>
       <c r="K18" s="29"/>
       <c r="L18" s="29"/>
       <c r="M18" s="29"/>
     </row>
-    <row r="19" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="105" x14ac:dyDescent="0.25">
       <c r="B19" s="27">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E19" s="28" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="G19" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="H19" s="30" t="s">
-        <v>73</v>
+        <v>14</v>
+      </c>
+      <c r="H19" s="29" t="s">
+        <v>7</v>
       </c>
       <c r="I19" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J19" s="29"/>
+      <c r="J19" s="29" t="s">
+        <v>7</v>
+      </c>
       <c r="K19" s="29"/>
       <c r="L19" s="29"/>
       <c r="M19" s="29"/>
     </row>
     <row r="20" spans="2:13" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="27">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="28" t="s">
         <v>68</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E20" s="28" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F20" s="28" t="s">
         <v>71</v>
       </c>
       <c r="G20" s="28" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="H20" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I20" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="J20" s="29"/>
+      <c r="J20" s="29" t="s">
+        <v>7</v>
+      </c>
       <c r="K20" s="29"/>
       <c r="L20" s="29"/>
       <c r="M20" s="29"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="31"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="31"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="31"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="32"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="33"/>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="31"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="J25" s="33"/>
-      <c r="K25" s="33"/>
-      <c r="L25" s="33"/>
-      <c r="M25" s="33"/>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26" s="31"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="33"/>
-      <c r="L26" s="33"/>
-      <c r="M26" s="33"/>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B27" s="31"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
+    <row r="21" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="B21" s="27">
+        <v>19</v>
+      </c>
+      <c r="C21" s="71" t="s">
+        <v>202</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="H21" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I21" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+    </row>
+    <row r="22" spans="2:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="B22" s="27">
+        <v>20</v>
+      </c>
+      <c r="C22" s="71" t="s">
+        <v>203</v>
+      </c>
+      <c r="D22" s="71" t="s">
+        <v>204</v>
+      </c>
+      <c r="E22" s="71" t="s">
+        <v>205</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="J22" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+    </row>
+    <row r="23" spans="2:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="B23" s="27">
+        <v>21</v>
+      </c>
+      <c r="C23" s="71" t="s">
+        <v>206</v>
+      </c>
+      <c r="D23" s="71" t="s">
+        <v>207</v>
+      </c>
+      <c r="E23" s="71" t="s">
+        <v>208</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="J23" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+    </row>
+    <row r="24" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="B24" s="27">
+        <v>22</v>
+      </c>
+      <c r="C24" s="71" t="s">
+        <v>209</v>
+      </c>
+      <c r="D24" s="71" t="s">
+        <v>210</v>
+      </c>
+      <c r="E24" s="71" t="s">
+        <v>211</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="J24" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+    </row>
+    <row r="25" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="B25" s="27">
+        <v>23</v>
+      </c>
+      <c r="C25" s="71" t="s">
+        <v>215</v>
+      </c>
+      <c r="D25" s="71" t="s">
+        <v>216</v>
+      </c>
+      <c r="E25" s="71" t="s">
+        <v>217</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="J25" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+    </row>
+    <row r="26" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="B26" s="27">
+        <v>24</v>
+      </c>
+      <c r="C26" s="71" t="s">
+        <v>212</v>
+      </c>
+      <c r="D26" s="71" t="s">
+        <v>213</v>
+      </c>
+      <c r="E26" s="71" t="s">
+        <v>214</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="J26" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+    </row>
+    <row r="27" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B28" s="31"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="33"/>
-      <c r="L28" s="33"/>
-      <c r="M28" s="33"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="31"/>
@@ -2178,6 +2371,104 @@
       <c r="K29" s="33"/>
       <c r="L29" s="33"/>
       <c r="M29" s="33"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="31"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="33"/>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="31"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="33"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="31"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="33"/>
+      <c r="I32" s="33"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="31"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="33"/>
+      <c r="I33" s="33"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" s="31"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="33"/>
+      <c r="L34" s="33"/>
+      <c r="M34" s="33"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" s="31"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="33"/>
+      <c r="J35" s="33"/>
+      <c r="K35" s="33"/>
+      <c r="L35" s="33"/>
+      <c r="M35" s="33"/>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="31"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="33"/>
+      <c r="J36" s="33"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="33"/>
+      <c r="M36" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2198,8 +2489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19A71C0E-D987-4F72-8E55-1A15A93E3B4A}">
   <dimension ref="B1:L32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2216,41 +2507,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="54" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="44"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="44"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="55"/>
       <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
@@ -2272,24 +2563,26 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="5"/>
+      <c r="I3" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -2299,24 +2592,26 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="5"/>
+      <c r="I4" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
@@ -2326,24 +2621,26 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="5"/>
+      <c r="I5" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
@@ -2353,24 +2650,26 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>99</v>
+        <v>114</v>
+      </c>
+      <c r="D6" s="71" t="s">
+        <v>219</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="5"/>
+      <c r="I6" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
@@ -2380,24 +2679,26 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="5"/>
+      <c r="I7" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
@@ -2407,24 +2708,26 @@
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="5"/>
+      <c r="I8" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -2434,24 +2737,26 @@
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>92</v>
-      </c>
       <c r="F9" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="5"/>
+      <c r="I9" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
@@ -2461,24 +2766,26 @@
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -2488,24 +2795,26 @@
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="5"/>
+      <c r="I11" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
@@ -2515,24 +2824,26 @@
         <v>10</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="5"/>
+      <c r="I12" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
@@ -2542,24 +2853,26 @@
         <v>11</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I13" s="5"/>
+        <v>72</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
@@ -2569,24 +2882,26 @@
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="5"/>
+      <c r="I14" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
@@ -2880,7 +3195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E40AF5E-F2E2-48FF-97C9-372CD64636EE}">
   <dimension ref="B1:L32"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H13" sqref="H3:H13"/>
     </sheetView>
   </sheetViews>
@@ -2898,41 +3213,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="D1" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="62" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="I1" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="50"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
       <c r="H2" s="15" t="s">
         <v>16</v>
       </c>
@@ -2954,25 +3269,25 @@
         <v>1</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J3" s="20"/>
       <c r="K3" s="20"/>
@@ -2983,25 +3298,25 @@
         <v>2</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E4" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="F4" s="22" t="s">
-        <v>133</v>
-      </c>
       <c r="G4" s="22" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
@@ -3012,25 +3327,25 @@
         <v>3</v>
       </c>
       <c r="C5" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="E5" s="18" t="s">
+      <c r="F5" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="F5" s="22" t="s">
-        <v>133</v>
-      </c>
       <c r="G5" s="22" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
@@ -3041,25 +3356,25 @@
         <v>4</v>
       </c>
       <c r="C6" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="E6" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="H6" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>152</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="H6" s="19" t="s">
-        <v>143</v>
-      </c>
       <c r="I6" s="20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J6" s="20"/>
       <c r="K6" s="20"/>
@@ -3070,25 +3385,25 @@
         <v>5</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H7" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
@@ -3099,25 +3414,25 @@
         <v>6</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J8" s="20"/>
       <c r="K8" s="20"/>
@@ -3128,25 +3443,25 @@
         <v>7</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
@@ -3157,25 +3472,25 @@
         <v>8</v>
       </c>
       <c r="C10" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="D10" s="23" t="s">
-        <v>148</v>
-      </c>
       <c r="E10" s="18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J10" s="20"/>
       <c r="K10" s="20"/>
@@ -3186,25 +3501,25 @@
         <v>9</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D11" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="E11" s="18" t="s">
-        <v>153</v>
-      </c>
       <c r="F11" s="22" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
@@ -3215,25 +3530,25 @@
         <v>10</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G12" s="22" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H12" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I12" s="20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J12" s="20"/>
       <c r="K12" s="20"/>
@@ -3244,25 +3559,25 @@
         <v>11</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D13" s="23" t="s">
+        <v>145</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="E13" s="18" t="s">
-        <v>151</v>
-      </c>
       <c r="F13" s="22" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H13" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I13" s="20" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
@@ -3572,707 +3887,707 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F34C6A-AD13-489E-B8D1-D0228FED8348}">
   <dimension ref="B1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="59" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="59"/>
-    <col min="3" max="3" width="28.140625" style="59" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="59" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="59" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="59" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="59" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="10.140625" style="59" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7109375" style="59"/>
+    <col min="1" max="1" width="3.28515625" style="36" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="36"/>
+    <col min="3" max="3" width="28.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="36" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="10.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7109375" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="68" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="56" t="s">
+      <c r="H1" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="I1" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="60"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="56" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="56" t="s">
+      <c r="I2" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="56" t="s">
+      <c r="J2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="56" t="s">
+      <c r="K2" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="56" t="s">
+      <c r="L2" s="35" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="2:12" ht="255" x14ac:dyDescent="0.25">
-      <c r="B3" s="62">
+      <c r="B3" s="37">
         <v>1</v>
       </c>
-      <c r="C3" s="63" t="s">
-        <v>122</v>
-      </c>
-      <c r="D3" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="E3" s="65" t="s">
+      <c r="C3" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="I3" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="42"/>
+      <c r="K3" s="42"/>
+      <c r="L3" s="42"/>
+    </row>
+    <row r="4" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="B4" s="37">
+        <v>2</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="40" t="s">
         <v>166</v>
       </c>
-      <c r="F3" s="65" t="s">
-        <v>124</v>
-      </c>
-      <c r="G3" s="65" t="s">
+      <c r="G4" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="I4" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+    </row>
+    <row r="5" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="B5" s="37">
+        <v>3</v>
+      </c>
+      <c r="C5" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="F5" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="G5" s="40" t="s">
         <v>167</v>
       </c>
-      <c r="H3" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="I3" s="67" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
-    </row>
-    <row r="4" spans="2:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="B4" s="62">
-        <v>2</v>
-      </c>
-      <c r="C4" s="68" t="s">
+      <c r="H5" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="I5" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+    </row>
+    <row r="6" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="B6" s="37">
+        <v>4</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="40" t="s">
         <v>171</v>
       </c>
-      <c r="D4" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="E4" s="65" t="s">
+      <c r="F6" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="G6" s="40" t="s">
         <v>172</v>
       </c>
-      <c r="F4" s="65" t="s">
-        <v>169</v>
-      </c>
-      <c r="G4" s="65" t="s">
+      <c r="H6" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="I6" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
+    </row>
+    <row r="7" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="B7" s="37">
+        <v>5</v>
+      </c>
+      <c r="C7" s="43" t="s">
         <v>173</v>
       </c>
-      <c r="H4" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="I4" s="67" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-    </row>
-    <row r="5" spans="2:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="B5" s="62">
-        <v>3</v>
-      </c>
-      <c r="C5" s="68" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="E5" s="65" t="s">
-        <v>168</v>
-      </c>
-      <c r="F5" s="65" t="s">
-        <v>169</v>
-      </c>
-      <c r="G5" s="65" t="s">
-        <v>170</v>
-      </c>
-      <c r="H5" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="I5" s="67" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="67"/>
-      <c r="K5" s="67"/>
-      <c r="L5" s="67"/>
-    </row>
-    <row r="6" spans="2:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="B6" s="62">
-        <v>4</v>
-      </c>
-      <c r="C6" s="68" t="s">
+      <c r="D7" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="D6" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="E6" s="65" t="s">
+      <c r="E7" s="40" t="s">
         <v>174</v>
       </c>
-      <c r="F6" s="65" t="s">
+      <c r="F7" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="H7" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="I7" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+    </row>
+    <row r="8" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="B8" s="37">
+        <v>5</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="F8" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="I8" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
+    </row>
+    <row r="9" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="B9" s="37">
+        <v>6</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>176</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="F9" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="G9" s="40" t="s">
         <v>181</v>
       </c>
-      <c r="G6" s="65" t="s">
-        <v>175</v>
-      </c>
-      <c r="H6" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="I6" s="67" t="s">
-        <v>7</v>
-      </c>
-      <c r="J6" s="67"/>
-      <c r="K6" s="67"/>
-      <c r="L6" s="67"/>
-    </row>
-    <row r="7" spans="2:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="B7" s="62">
-        <v>5</v>
-      </c>
-      <c r="C7" s="68" t="s">
+      <c r="H9" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="I9" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+    </row>
+    <row r="10" spans="2:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="B10" s="37">
+        <v>7</v>
+      </c>
+      <c r="C10" s="43" t="s">
         <v>176</v>
       </c>
-      <c r="D7" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" s="65" t="s">
-        <v>177</v>
-      </c>
-      <c r="F7" s="65" t="s">
-        <v>181</v>
-      </c>
-      <c r="G7" s="65" t="s">
-        <v>178</v>
-      </c>
-      <c r="H7" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="I7" s="67" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" s="67"/>
-      <c r="K7" s="67"/>
-      <c r="L7" s="67"/>
-    </row>
-    <row r="8" spans="2:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="B8" s="62">
-        <v>5</v>
-      </c>
-      <c r="C8" s="68" t="s">
-        <v>179</v>
-      </c>
-      <c r="D8" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="E8" s="65" t="s">
-        <v>180</v>
-      </c>
-      <c r="F8" s="65" t="s">
-        <v>181</v>
-      </c>
-      <c r="G8" s="65" t="s">
+      <c r="D10" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" s="40" t="s">
         <v>182</v>
       </c>
-      <c r="H8" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="I8" s="67" t="s">
-        <v>7</v>
-      </c>
-      <c r="J8" s="67"/>
-      <c r="K8" s="67"/>
-      <c r="L8" s="67"/>
-    </row>
-    <row r="9" spans="2:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="B9" s="62">
-        <v>6</v>
-      </c>
-      <c r="C9" s="68" t="s">
-        <v>179</v>
-      </c>
-      <c r="D9" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="E9" s="65" t="s">
+      <c r="F10" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="F9" s="65" t="s">
-        <v>181</v>
-      </c>
-      <c r="G9" s="65" t="s">
+      <c r="G10" s="40" t="s">
         <v>184</v>
       </c>
-      <c r="H9" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="I9" s="67" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="67"/>
-      <c r="K9" s="67"/>
-      <c r="L9" s="67"/>
-    </row>
-    <row r="10" spans="2:12" ht="105" x14ac:dyDescent="0.25">
-      <c r="B10" s="62">
-        <v>7</v>
-      </c>
-      <c r="C10" s="68" t="s">
-        <v>179</v>
-      </c>
-      <c r="D10" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="E10" s="65" t="s">
+      <c r="H10" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="I10" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+    </row>
+    <row r="11" spans="2:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="B11" s="37">
+        <v>8</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>188</v>
+      </c>
+      <c r="D11" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="F11" s="40" t="s">
         <v>185</v>
       </c>
-      <c r="F10" s="65" t="s">
-        <v>186</v>
-      </c>
-      <c r="G10" s="65" t="s">
+      <c r="G11" s="45" t="s">
         <v>187</v>
       </c>
-      <c r="H10" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="I10" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-    </row>
-    <row r="11" spans="2:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="B11" s="62">
-        <v>8</v>
-      </c>
-      <c r="C11" s="65" t="s">
+      <c r="H11" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="I11" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+    </row>
+    <row r="12" spans="2:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="B12" s="37">
+        <v>9</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="F12" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="G12" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="H12" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="I12" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+    </row>
+    <row r="13" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="B13" s="37">
+        <v>10</v>
+      </c>
+      <c r="C13" s="43" t="s">
+        <v>192</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="F13" s="45" t="s">
         <v>191</v>
       </c>
-      <c r="D11" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="E11" s="65" t="s">
-        <v>189</v>
-      </c>
-      <c r="F11" s="65" t="s">
-        <v>188</v>
-      </c>
-      <c r="G11" s="70" t="s">
-        <v>190</v>
-      </c>
-      <c r="H11" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="I11" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="J11" s="67"/>
-      <c r="K11" s="67"/>
-      <c r="L11" s="67"/>
-    </row>
-    <row r="12" spans="2:12" ht="120" x14ac:dyDescent="0.25">
-      <c r="B12" s="62">
-        <v>9</v>
-      </c>
-      <c r="C12" s="65" t="s">
-        <v>192</v>
-      </c>
-      <c r="D12" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="E12" s="65" t="s">
+      <c r="G13" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="I13" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
+    </row>
+    <row r="14" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="B14" s="37">
+        <v>11</v>
+      </c>
+      <c r="C14" s="43" t="s">
+        <v>196</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="E14" s="40" t="s">
         <v>193</v>
       </c>
-      <c r="F12" s="65" t="s">
-        <v>188</v>
-      </c>
-      <c r="G12" s="70" t="s">
-        <v>190</v>
-      </c>
-      <c r="H12" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="I12" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="J12" s="67"/>
-      <c r="K12" s="67"/>
-      <c r="L12" s="67"/>
-    </row>
-    <row r="13" spans="2:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="B13" s="62">
-        <v>10</v>
-      </c>
-      <c r="C13" s="68" t="s">
+      <c r="F14" s="45" t="s">
+        <v>191</v>
+      </c>
+      <c r="G14" s="45" t="s">
         <v>195</v>
       </c>
-      <c r="D13" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="E13" s="65" t="s">
-        <v>197</v>
-      </c>
-      <c r="F13" s="70" t="s">
-        <v>194</v>
-      </c>
-      <c r="G13" s="70" t="s">
-        <v>198</v>
-      </c>
-      <c r="H13" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="I13" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="J13" s="67"/>
-      <c r="K13" s="67"/>
-      <c r="L13" s="67"/>
-    </row>
-    <row r="14" spans="2:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="B14" s="62">
-        <v>11</v>
-      </c>
-      <c r="C14" s="68" t="s">
-        <v>199</v>
-      </c>
-      <c r="D14" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="E14" s="65" t="s">
-        <v>196</v>
-      </c>
-      <c r="F14" s="70" t="s">
-        <v>194</v>
-      </c>
-      <c r="G14" s="70" t="s">
-        <v>198</v>
-      </c>
-      <c r="H14" s="66" t="s">
-        <v>143</v>
-      </c>
-      <c r="I14" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="J14" s="67"/>
-      <c r="K14" s="67"/>
-      <c r="L14" s="67"/>
+      <c r="H14" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="I14" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="62">
+      <c r="B15" s="37">
         <v>12</v>
       </c>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="67"/>
-      <c r="J15" s="67"/>
-      <c r="K15" s="67"/>
-      <c r="L15" s="67"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="62">
+      <c r="B16" s="37">
         <v>13</v>
       </c>
-      <c r="C16" s="70"/>
-      <c r="D16" s="70"/>
-      <c r="E16" s="70"/>
-      <c r="F16" s="70"/>
-      <c r="G16" s="70"/>
-      <c r="H16" s="67"/>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="67"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="62">
+      <c r="B17" s="37">
         <v>14</v>
       </c>
-      <c r="C17" s="70"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="70"/>
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
-      <c r="K17" s="67"/>
-      <c r="L17" s="67"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="62">
+      <c r="B18" s="37">
         <v>15</v>
       </c>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
-      <c r="K18" s="67"/>
-      <c r="L18" s="67"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="42"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="62">
+      <c r="B19" s="37">
         <v>16</v>
       </c>
-      <c r="C19" s="70"/>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="70"/>
-      <c r="G19" s="70"/>
-      <c r="H19" s="67"/>
-      <c r="I19" s="67"/>
-      <c r="J19" s="67"/>
-      <c r="K19" s="67"/>
-      <c r="L19" s="67"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="42"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="62">
+      <c r="B20" s="37">
         <v>17</v>
       </c>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="70"/>
-      <c r="F20" s="70"/>
-      <c r="G20" s="70"/>
-      <c r="H20" s="67"/>
-      <c r="I20" s="67"/>
-      <c r="J20" s="67"/>
-      <c r="K20" s="67"/>
-      <c r="L20" s="67"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="42"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B21" s="62">
+      <c r="B21" s="37">
         <v>18</v>
       </c>
-      <c r="C21" s="70"/>
-      <c r="D21" s="70"/>
-      <c r="E21" s="70"/>
-      <c r="F21" s="70"/>
-      <c r="G21" s="70"/>
-      <c r="H21" s="67"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="67"/>
-      <c r="K21" s="67"/>
-      <c r="L21" s="67"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="42"/>
+      <c r="L21" s="42"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="62">
+      <c r="B22" s="37">
         <v>19</v>
       </c>
-      <c r="C22" s="70"/>
-      <c r="D22" s="70"/>
-      <c r="E22" s="70"/>
-      <c r="F22" s="70"/>
-      <c r="G22" s="70"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="67"/>
-      <c r="J22" s="67"/>
-      <c r="K22" s="67"/>
-      <c r="L22" s="67"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="62">
+      <c r="B23" s="37">
         <v>20</v>
       </c>
-      <c r="C23" s="70"/>
-      <c r="D23" s="70"/>
-      <c r="E23" s="70"/>
-      <c r="F23" s="70"/>
-      <c r="G23" s="70"/>
-      <c r="H23" s="67"/>
-      <c r="I23" s="67"/>
-      <c r="J23" s="67"/>
-      <c r="K23" s="67"/>
-      <c r="L23" s="67"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="42"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="62">
+      <c r="B24" s="37">
         <v>21</v>
       </c>
-      <c r="C24" s="70"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="70"/>
-      <c r="F24" s="70"/>
-      <c r="G24" s="70"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
-      <c r="K24" s="67"/>
-      <c r="L24" s="67"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="62">
+      <c r="B25" s="37">
         <v>22</v>
       </c>
-      <c r="C25" s="70"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="70"/>
-      <c r="F25" s="70"/>
-      <c r="G25" s="70"/>
-      <c r="H25" s="67"/>
-      <c r="I25" s="67"/>
-      <c r="J25" s="67"/>
-      <c r="K25" s="67"/>
-      <c r="L25" s="67"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="62">
+      <c r="B26" s="37">
         <v>23</v>
       </c>
-      <c r="C26" s="70"/>
-      <c r="D26" s="70"/>
-      <c r="E26" s="70"/>
-      <c r="F26" s="70"/>
-      <c r="G26" s="70"/>
-      <c r="H26" s="67"/>
-      <c r="I26" s="67"/>
-      <c r="J26" s="67"/>
-      <c r="K26" s="67"/>
-      <c r="L26" s="67"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="62">
+      <c r="B27" s="37">
         <v>24</v>
       </c>
-      <c r="C27" s="70"/>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="70"/>
-      <c r="H27" s="67"/>
-      <c r="I27" s="67"/>
-      <c r="J27" s="67"/>
-      <c r="K27" s="67"/>
-      <c r="L27" s="67"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="42"/>
+      <c r="L27" s="42"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="62">
+      <c r="B28" s="37">
         <v>25</v>
       </c>
-      <c r="C28" s="70"/>
-      <c r="D28" s="70"/>
-      <c r="E28" s="70"/>
-      <c r="F28" s="70"/>
-      <c r="G28" s="70"/>
-      <c r="H28" s="67"/>
-      <c r="I28" s="67"/>
-      <c r="J28" s="67"/>
-      <c r="K28" s="67"/>
-      <c r="L28" s="67"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="42"/>
+      <c r="L28" s="42"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="62">
+      <c r="B29" s="37">
         <v>26</v>
       </c>
-      <c r="C29" s="70"/>
-      <c r="D29" s="70"/>
-      <c r="E29" s="70"/>
-      <c r="F29" s="70"/>
-      <c r="G29" s="70"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="67"/>
-      <c r="J29" s="67"/>
-      <c r="K29" s="67"/>
-      <c r="L29" s="67"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="42"/>
+      <c r="I29" s="42"/>
+      <c r="J29" s="42"/>
+      <c r="K29" s="42"/>
+      <c r="L29" s="42"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="62">
+      <c r="B30" s="37">
         <v>27</v>
       </c>
-      <c r="C30" s="70"/>
-      <c r="D30" s="70"/>
-      <c r="E30" s="70"/>
-      <c r="F30" s="70"/>
-      <c r="G30" s="70"/>
-      <c r="H30" s="67"/>
-      <c r="I30" s="67"/>
-      <c r="J30" s="67"/>
-      <c r="K30" s="67"/>
-      <c r="L30" s="67"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="42"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="42"/>
+      <c r="L30" s="42"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="62">
+      <c r="B31" s="37">
         <v>28</v>
       </c>
-      <c r="C31" s="70"/>
-      <c r="D31" s="70"/>
-      <c r="E31" s="70"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="70"/>
-      <c r="H31" s="67"/>
-      <c r="I31" s="67"/>
-      <c r="J31" s="67"/>
-      <c r="K31" s="67"/>
-      <c r="L31" s="67"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="42"/>
+      <c r="L31" s="42"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="62">
+      <c r="B32" s="37">
         <v>29</v>
       </c>
-      <c r="C32" s="70"/>
-      <c r="D32" s="70"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="70"/>
-      <c r="G32" s="70"/>
-      <c r="H32" s="67"/>
-      <c r="I32" s="67"/>
-      <c r="J32" s="67"/>
-      <c r="K32" s="67"/>
-      <c r="L32" s="67"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="42"/>
+      <c r="L32" s="42"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="62">
+      <c r="B33" s="37">
         <v>30</v>
       </c>
-      <c r="C33" s="70"/>
-      <c r="D33" s="70"/>
-      <c r="E33" s="70"/>
-      <c r="F33" s="70"/>
-      <c r="G33" s="70"/>
-      <c r="H33" s="67"/>
-      <c r="I33" s="67"/>
-      <c r="J33" s="67"/>
-      <c r="K33" s="67"/>
-      <c r="L33" s="67"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="42"/>
+      <c r="J33" s="42"/>
+      <c r="K33" s="42"/>
+      <c r="L33" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -4311,41 +4626,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="70" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="I1" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
       <c r="H2" s="7" t="s">
         <v>16</v>
       </c>
@@ -4367,16 +4682,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="12"/>
@@ -4390,16 +4705,16 @@
         <v>2</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>162</v>
-      </c>
       <c r="F4" s="10" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="12"/>
@@ -4413,16 +4728,16 @@
         <v>3</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="E5" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>161</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>164</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="12"/>

</xml_diff>

<commit_message>
Test case iteration update missing results
</commit_message>
<xml_diff>
--- a/testing/Testcases-iteration.xlsx
+++ b/testing/Testcases-iteration.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel Tay\Desktop\SMU\SEM 2.1\SE\SE Project\is203-2017_G1T3\testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ming Xuan\Desktop\Year 2\SE\SE project\is203-2017_G1T3\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6945" tabRatio="1000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" tabRatio="1000" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case for Login Validation" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="222">
   <si>
     <t>S/N</t>
   </si>
@@ -734,6 +734,12 @@
   </si>
   <si>
     <t xml:space="preserve"> this-mixcase.zip</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -988,7 +994,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1117,6 +1123,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1192,8 +1201,8 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1515,56 +1524,56 @@
       <selection activeCell="H22" sqref="H22:H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="26" customWidth="1"/>
-    <col min="2" max="2" width="3.7109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="34" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="34" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="34" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="34" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" style="26" customWidth="1"/>
+    <col min="1" max="1" width="3.26953125" style="26" customWidth="1"/>
+    <col min="2" max="2" width="3.7265625" style="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.54296875" style="34" customWidth="1"/>
+    <col min="4" max="4" width="24.26953125" style="34" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" style="34" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" style="34" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.54296875" style="26" customWidth="1"/>
     <col min="8" max="12" width="10" style="26" customWidth="1"/>
-    <col min="13" max="16384" width="8.7109375" style="26"/>
+    <col min="13" max="16384" width="8.7265625" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B1" s="48" t="s">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="50" t="s">
+      <c r="F1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="49" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-    </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="49"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="49"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B2" s="50"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="25" t="s">
         <v>10</v>
       </c>
@@ -1584,7 +1593,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B3" s="27">
         <v>1</v>
       </c>
@@ -1616,7 +1625,7 @@
       <c r="L3" s="29"/>
       <c r="M3" s="29"/>
     </row>
-    <row r="4" spans="2:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B4" s="27">
         <v>2</v>
       </c>
@@ -1648,7 +1657,7 @@
       <c r="L4" s="29"/>
       <c r="M4" s="29"/>
     </row>
-    <row r="5" spans="2:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" ht="58" x14ac:dyDescent="0.35">
       <c r="B5" s="27">
         <v>3</v>
       </c>
@@ -1661,10 +1670,10 @@
       <c r="E5" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="71" t="s">
+      <c r="F5" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="G5" s="71" t="s">
+      <c r="G5" s="46" t="s">
         <v>200</v>
       </c>
       <c r="H5" s="29" t="s">
@@ -1680,7 +1689,7 @@
       <c r="L5" s="29"/>
       <c r="M5" s="29"/>
     </row>
-    <row r="6" spans="2:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B6" s="27">
         <v>4</v>
       </c>
@@ -1712,7 +1721,7 @@
       <c r="L6" s="29"/>
       <c r="M6" s="29"/>
     </row>
-    <row r="7" spans="2:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B7" s="27">
         <v>5</v>
       </c>
@@ -1744,7 +1753,7 @@
       <c r="L7" s="29"/>
       <c r="M7" s="29"/>
     </row>
-    <row r="8" spans="2:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" ht="58" x14ac:dyDescent="0.35">
       <c r="B8" s="27">
         <v>6</v>
       </c>
@@ -1757,10 +1766,10 @@
       <c r="E8" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="71" t="s">
+      <c r="F8" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="G8" s="71" t="s">
+      <c r="G8" s="46" t="s">
         <v>200</v>
       </c>
       <c r="H8" s="29" t="s">
@@ -1776,7 +1785,7 @@
       <c r="L8" s="29"/>
       <c r="M8" s="29"/>
     </row>
-    <row r="9" spans="2:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="58" x14ac:dyDescent="0.35">
       <c r="B9" s="27">
         <v>7</v>
       </c>
@@ -1789,10 +1798,10 @@
       <c r="E9" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="71" t="s">
+      <c r="F9" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="G9" s="71" t="s">
+      <c r="G9" s="46" t="s">
         <v>200</v>
       </c>
       <c r="H9" s="29" t="s">
@@ -1808,7 +1817,7 @@
       <c r="L9" s="29"/>
       <c r="M9" s="29"/>
     </row>
-    <row r="10" spans="2:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B10" s="27">
         <v>8</v>
       </c>
@@ -1840,7 +1849,7 @@
       <c r="L10" s="29"/>
       <c r="M10" s="29"/>
     </row>
-    <row r="11" spans="2:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" ht="58" x14ac:dyDescent="0.35">
       <c r="B11" s="27">
         <v>9</v>
       </c>
@@ -1853,10 +1862,10 @@
       <c r="E11" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="71" t="s">
+      <c r="F11" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="G11" s="71" t="s">
+      <c r="G11" s="46" t="s">
         <v>200</v>
       </c>
       <c r="H11" s="29" t="s">
@@ -1872,23 +1881,23 @@
       <c r="L11" s="29"/>
       <c r="M11" s="29"/>
     </row>
-    <row r="12" spans="2:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="58" x14ac:dyDescent="0.35">
       <c r="B12" s="27">
         <v>10</v>
       </c>
-      <c r="C12" s="71" t="s">
+      <c r="C12" s="46" t="s">
         <v>197</v>
       </c>
-      <c r="D12" s="71" t="s">
+      <c r="D12" s="46" t="s">
         <v>198</v>
       </c>
-      <c r="E12" s="71" t="s">
+      <c r="E12" s="46" t="s">
         <v>199</v>
       </c>
-      <c r="F12" s="71" t="s">
+      <c r="F12" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="G12" s="71" t="s">
+      <c r="G12" s="46" t="s">
         <v>200</v>
       </c>
       <c r="H12" s="29"/>
@@ -1898,7 +1907,7 @@
       <c r="L12" s="29"/>
       <c r="M12" s="29"/>
     </row>
-    <row r="13" spans="2:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B13" s="27">
         <v>11</v>
       </c>
@@ -1930,7 +1939,7 @@
       <c r="L13" s="29"/>
       <c r="M13" s="29"/>
     </row>
-    <row r="14" spans="2:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B14" s="27">
         <v>12</v>
       </c>
@@ -1962,7 +1971,7 @@
       <c r="L14" s="29"/>
       <c r="M14" s="29"/>
     </row>
-    <row r="15" spans="2:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" ht="87" x14ac:dyDescent="0.35">
       <c r="B15" s="27">
         <v>13</v>
       </c>
@@ -1975,10 +1984,10 @@
       <c r="E15" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="71" t="s">
+      <c r="F15" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="G15" s="71" t="s">
+      <c r="G15" s="46" t="s">
         <v>200</v>
       </c>
       <c r="H15" s="29" t="s">
@@ -1994,7 +2003,7 @@
       <c r="L15" s="29"/>
       <c r="M15" s="29"/>
     </row>
-    <row r="16" spans="2:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" ht="87" x14ac:dyDescent="0.35">
       <c r="B16" s="27">
         <v>14</v>
       </c>
@@ -2026,7 +2035,7 @@
       <c r="L16" s="29"/>
       <c r="M16" s="29"/>
     </row>
-    <row r="17" spans="2:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" ht="58" x14ac:dyDescent="0.35">
       <c r="B17" s="27">
         <v>15</v>
       </c>
@@ -2039,10 +2048,10 @@
       <c r="E17" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="71" t="s">
+      <c r="F17" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="G17" s="71" t="s">
+      <c r="G17" s="46" t="s">
         <v>200</v>
       </c>
       <c r="H17" s="29" t="s">
@@ -2058,7 +2067,7 @@
       <c r="L17" s="29"/>
       <c r="M17" s="29"/>
     </row>
-    <row r="18" spans="2:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" ht="87" x14ac:dyDescent="0.35">
       <c r="B18" s="27">
         <v>16</v>
       </c>
@@ -2090,7 +2099,7 @@
       <c r="L18" s="29"/>
       <c r="M18" s="29"/>
     </row>
-    <row r="19" spans="2:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" ht="87" x14ac:dyDescent="0.35">
       <c r="B19" s="27">
         <v>17</v>
       </c>
@@ -2122,7 +2131,7 @@
       <c r="L19" s="29"/>
       <c r="M19" s="29"/>
     </row>
-    <row r="20" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B20" s="27">
         <v>18</v>
       </c>
@@ -2154,11 +2163,11 @@
       <c r="L20" s="29"/>
       <c r="M20" s="29"/>
     </row>
-    <row r="21" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B21" s="27">
         <v>19</v>
       </c>
-      <c r="C21" s="71" t="s">
+      <c r="C21" s="46" t="s">
         <v>202</v>
       </c>
       <c r="D21" s="28" t="s">
@@ -2186,17 +2195,17 @@
       <c r="L21" s="29"/>
       <c r="M21" s="29"/>
     </row>
-    <row r="22" spans="2:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B22" s="27">
         <v>20</v>
       </c>
-      <c r="C22" s="71" t="s">
+      <c r="C22" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="D22" s="71" t="s">
+      <c r="D22" s="46" t="s">
         <v>204</v>
       </c>
-      <c r="E22" s="71" t="s">
+      <c r="E22" s="46" t="s">
         <v>205</v>
       </c>
       <c r="F22" s="28" t="s">
@@ -2218,17 +2227,17 @@
       <c r="L22" s="29"/>
       <c r="M22" s="29"/>
     </row>
-    <row r="23" spans="2:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B23" s="27">
         <v>21</v>
       </c>
-      <c r="C23" s="71" t="s">
+      <c r="C23" s="46" t="s">
         <v>206</v>
       </c>
-      <c r="D23" s="71" t="s">
+      <c r="D23" s="46" t="s">
         <v>207</v>
       </c>
-      <c r="E23" s="71" t="s">
+      <c r="E23" s="46" t="s">
         <v>208</v>
       </c>
       <c r="F23" s="28" t="s">
@@ -2250,17 +2259,17 @@
       <c r="L23" s="29"/>
       <c r="M23" s="29"/>
     </row>
-    <row r="24" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" ht="58" x14ac:dyDescent="0.35">
       <c r="B24" s="27">
         <v>22</v>
       </c>
-      <c r="C24" s="71" t="s">
+      <c r="C24" s="46" t="s">
         <v>209</v>
       </c>
-      <c r="D24" s="71" t="s">
+      <c r="D24" s="46" t="s">
         <v>210</v>
       </c>
-      <c r="E24" s="71" t="s">
+      <c r="E24" s="46" t="s">
         <v>211</v>
       </c>
       <c r="F24" s="28" t="s">
@@ -2282,17 +2291,17 @@
       <c r="L24" s="29"/>
       <c r="M24" s="29"/>
     </row>
-    <row r="25" spans="2:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" ht="58" x14ac:dyDescent="0.35">
       <c r="B25" s="27">
         <v>23</v>
       </c>
-      <c r="C25" s="71" t="s">
+      <c r="C25" s="46" t="s">
         <v>215</v>
       </c>
-      <c r="D25" s="71" t="s">
+      <c r="D25" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="E25" s="71" t="s">
+      <c r="E25" s="46" t="s">
         <v>217</v>
       </c>
       <c r="F25" s="28" t="s">
@@ -2314,17 +2323,17 @@
       <c r="L25" s="29"/>
       <c r="M25" s="29"/>
     </row>
-    <row r="26" spans="2:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B26" s="27">
         <v>24</v>
       </c>
-      <c r="C26" s="71" t="s">
+      <c r="C26" s="46" t="s">
         <v>212</v>
       </c>
-      <c r="D26" s="71" t="s">
+      <c r="D26" s="46" t="s">
         <v>213</v>
       </c>
-      <c r="E26" s="71" t="s">
+      <c r="E26" s="46" t="s">
         <v>214</v>
       </c>
       <c r="F26" s="28" t="s">
@@ -2346,19 +2355,19 @@
       <c r="L26" s="29"/>
       <c r="M26" s="29"/>
     </row>
-    <row r="27" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C27" s="26"/>
       <c r="D27" s="26"/>
       <c r="E27" s="26"/>
       <c r="F27" s="26"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C28" s="26"/>
       <c r="D28" s="26"/>
       <c r="E28" s="26"/>
       <c r="F28" s="26"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B29" s="31"/>
       <c r="C29" s="32"/>
       <c r="D29" s="32"/>
@@ -2372,7 +2381,7 @@
       <c r="L29" s="33"/>
       <c r="M29" s="33"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B30" s="31"/>
       <c r="C30" s="32"/>
       <c r="D30" s="32"/>
@@ -2386,7 +2395,7 @@
       <c r="L30" s="33"/>
       <c r="M30" s="33"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B31" s="31"/>
       <c r="C31" s="32"/>
       <c r="D31" s="32"/>
@@ -2400,7 +2409,7 @@
       <c r="L31" s="33"/>
       <c r="M31" s="33"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B32" s="31"/>
       <c r="C32" s="32"/>
       <c r="D32" s="32"/>
@@ -2414,7 +2423,7 @@
       <c r="L32" s="33"/>
       <c r="M32" s="33"/>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B33" s="31"/>
       <c r="C33" s="32"/>
       <c r="D33" s="32"/>
@@ -2428,7 +2437,7 @@
       <c r="L33" s="33"/>
       <c r="M33" s="33"/>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B34" s="31"/>
       <c r="C34" s="32"/>
       <c r="D34" s="32"/>
@@ -2442,7 +2451,7 @@
       <c r="L34" s="33"/>
       <c r="M34" s="33"/>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B35" s="31"/>
       <c r="C35" s="32"/>
       <c r="D35" s="32"/>
@@ -2456,7 +2465,7 @@
       <c r="L35" s="33"/>
       <c r="M35" s="33"/>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B36" s="31"/>
       <c r="C36" s="32"/>
       <c r="D36" s="32"/>
@@ -2489,59 +2498,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19A71C0E-D987-4F72-8E55-1A15A93E3B4A}">
   <dimension ref="B1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:H7"/>
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="2"/>
-    <col min="3" max="3" width="25.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7109375" style="2"/>
+    <col min="1" max="1" width="3.26953125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="2"/>
+    <col min="3" max="3" width="25.1796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="28.54296875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="10.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="54" t="s">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="56" t="s">
+      <c r="F1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="55" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="55"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="55"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B2" s="56"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="56"/>
       <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
@@ -2558,7 +2567,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" ht="145" x14ac:dyDescent="0.35">
       <c r="B3" s="3">
         <v>1</v>
       </c>
@@ -2587,7 +2596,7 @@
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" ht="87" x14ac:dyDescent="0.35">
       <c r="B4" s="3">
         <v>2</v>
       </c>
@@ -2616,7 +2625,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="87" x14ac:dyDescent="0.35">
       <c r="B5" s="3">
         <v>3</v>
       </c>
@@ -2645,14 +2654,14 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="2:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="145" x14ac:dyDescent="0.35">
       <c r="B6" s="3">
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D6" s="71" t="s">
+      <c r="D6" s="46" t="s">
         <v>219</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -2674,7 +2683,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="2:12" ht="150" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" ht="130.5" x14ac:dyDescent="0.35">
       <c r="B7" s="3">
         <v>5</v>
       </c>
@@ -2703,7 +2712,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="87" x14ac:dyDescent="0.35">
       <c r="B8" s="3">
         <v>6</v>
       </c>
@@ -2732,7 +2741,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="2:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" ht="159.5" x14ac:dyDescent="0.35">
       <c r="B9" s="3">
         <v>7</v>
       </c>
@@ -2761,7 +2770,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="2:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" ht="159.5" x14ac:dyDescent="0.35">
       <c r="B10" s="3">
         <v>8</v>
       </c>
@@ -2790,7 +2799,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="2:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="145" x14ac:dyDescent="0.35">
       <c r="B11" s="3">
         <v>9</v>
       </c>
@@ -2819,7 +2828,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="2:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" ht="159.5" x14ac:dyDescent="0.35">
       <c r="B12" s="3">
         <v>10</v>
       </c>
@@ -2848,7 +2857,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="2:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="159.5" x14ac:dyDescent="0.35">
       <c r="B13" s="3">
         <v>11</v>
       </c>
@@ -2877,7 +2886,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="2:12" ht="165" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" ht="159.5" x14ac:dyDescent="0.35">
       <c r="B14" s="3">
         <v>12</v>
       </c>
@@ -2906,7 +2915,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B15" s="3">
         <v>13</v>
       </c>
@@ -2921,7 +2930,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="3">
         <v>14</v>
       </c>
@@ -2936,7 +2945,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B17" s="3">
         <v>15</v>
       </c>
@@ -2951,7 +2960,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18" s="3">
         <v>16</v>
       </c>
@@ -2966,7 +2975,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B19" s="3">
         <v>17</v>
       </c>
@@ -2981,7 +2990,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B20" s="3">
         <v>18</v>
       </c>
@@ -2996,7 +3005,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B21" s="3">
         <v>19</v>
       </c>
@@ -3011,7 +3020,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B22" s="3">
         <v>20</v>
       </c>
@@ -3026,7 +3035,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B23" s="3">
         <v>21</v>
       </c>
@@ -3041,7 +3050,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B24" s="3">
         <v>22</v>
       </c>
@@ -3056,7 +3065,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B25" s="3">
         <v>23</v>
       </c>
@@ -3071,7 +3080,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B26" s="3">
         <v>24</v>
       </c>
@@ -3086,7 +3095,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B27" s="3">
         <v>25</v>
       </c>
@@ -3101,7 +3110,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B28" s="3">
         <v>26</v>
       </c>
@@ -3116,7 +3125,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B29" s="3">
         <v>27</v>
       </c>
@@ -3131,7 +3140,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B30" s="3">
         <v>28</v>
       </c>
@@ -3146,7 +3155,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B31" s="3">
         <v>29</v>
       </c>
@@ -3161,7 +3170,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B32" s="3">
         <v>30</v>
       </c>
@@ -3199,55 +3208,55 @@
       <selection activeCell="H13" sqref="H3:H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="16"/>
-    <col min="3" max="3" width="28.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="16" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" style="16" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="24" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" style="24" customWidth="1"/>
-    <col min="8" max="12" width="10.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7109375" style="16"/>
+    <col min="1" max="1" width="3.26953125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="16"/>
+    <col min="3" max="3" width="28.1796875" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.54296875" style="16" customWidth="1"/>
+    <col min="5" max="5" width="25.81640625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="21.453125" style="24" customWidth="1"/>
+    <col min="7" max="7" width="20.1796875" style="24" customWidth="1"/>
+    <col min="8" max="12" width="10.1796875" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="60" t="s">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="62" t="s">
+      <c r="E1" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="F1" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="62" t="s">
+      <c r="G1" s="63" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="58" t="s">
+      <c r="I1" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="61"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B2" s="62"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
       <c r="H2" s="15" t="s">
         <v>16</v>
       </c>
@@ -3264,7 +3273,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B3" s="17">
         <v>1</v>
       </c>
@@ -3293,7 +3302,7 @@
       <c r="K3" s="20"/>
       <c r="L3" s="20"/>
     </row>
-    <row r="4" spans="2:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B4" s="17">
         <v>2</v>
       </c>
@@ -3322,7 +3331,7 @@
       <c r="K4" s="20"/>
       <c r="L4" s="20"/>
     </row>
-    <row r="5" spans="2:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B5" s="17">
         <v>3</v>
       </c>
@@ -3351,7 +3360,7 @@
       <c r="K5" s="20"/>
       <c r="L5" s="20"/>
     </row>
-    <row r="6" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B6" s="17">
         <v>4</v>
       </c>
@@ -3380,7 +3389,7 @@
       <c r="K6" s="20"/>
       <c r="L6" s="20"/>
     </row>
-    <row r="7" spans="2:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B7" s="17">
         <v>5</v>
       </c>
@@ -3409,7 +3418,7 @@
       <c r="K7" s="20"/>
       <c r="L7" s="20"/>
     </row>
-    <row r="8" spans="2:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B8" s="17">
         <v>6</v>
       </c>
@@ -3438,7 +3447,7 @@
       <c r="K8" s="20"/>
       <c r="L8" s="20"/>
     </row>
-    <row r="9" spans="2:12" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B9" s="17">
         <v>7</v>
       </c>
@@ -3467,7 +3476,7 @@
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
     </row>
-    <row r="10" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B10" s="17">
         <v>8</v>
       </c>
@@ -3496,7 +3505,7 @@
       <c r="K10" s="20"/>
       <c r="L10" s="20"/>
     </row>
-    <row r="11" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B11" s="17">
         <v>9</v>
       </c>
@@ -3525,7 +3534,7 @@
       <c r="K11" s="20"/>
       <c r="L11" s="20"/>
     </row>
-    <row r="12" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B12" s="17">
         <v>10</v>
       </c>
@@ -3554,7 +3563,7 @@
       <c r="K12" s="20"/>
       <c r="L12" s="20"/>
     </row>
-    <row r="13" spans="2:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="87" x14ac:dyDescent="0.35">
       <c r="B13" s="17">
         <v>11</v>
       </c>
@@ -3583,7 +3592,7 @@
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B14" s="17">
         <v>12</v>
       </c>
@@ -3598,7 +3607,7 @@
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B15" s="17">
         <v>13</v>
       </c>
@@ -3613,7 +3622,7 @@
       <c r="K15" s="20"/>
       <c r="L15" s="20"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="17">
         <v>14</v>
       </c>
@@ -3628,7 +3637,7 @@
       <c r="K16" s="20"/>
       <c r="L16" s="20"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B17" s="17">
         <v>15</v>
       </c>
@@ -3643,7 +3652,7 @@
       <c r="K17" s="20"/>
       <c r="L17" s="20"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18" s="17">
         <v>16</v>
       </c>
@@ -3658,7 +3667,7 @@
       <c r="K18" s="20"/>
       <c r="L18" s="20"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B19" s="17">
         <v>17</v>
       </c>
@@ -3673,7 +3682,7 @@
       <c r="K19" s="20"/>
       <c r="L19" s="20"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B20" s="17">
         <v>18</v>
       </c>
@@ -3688,7 +3697,7 @@
       <c r="K20" s="20"/>
       <c r="L20" s="20"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B21" s="17">
         <v>19</v>
       </c>
@@ -3703,7 +3712,7 @@
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B22" s="17">
         <v>20</v>
       </c>
@@ -3718,7 +3727,7 @@
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B23" s="17">
         <v>21</v>
       </c>
@@ -3733,7 +3742,7 @@
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B24" s="17">
         <v>22</v>
       </c>
@@ -3748,7 +3757,7 @@
       <c r="K24" s="20"/>
       <c r="L24" s="20"/>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B25" s="17">
         <v>23</v>
       </c>
@@ -3763,7 +3772,7 @@
       <c r="K25" s="20"/>
       <c r="L25" s="20"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B26" s="17">
         <v>24</v>
       </c>
@@ -3778,7 +3787,7 @@
       <c r="K26" s="20"/>
       <c r="L26" s="20"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B27" s="17">
         <v>25</v>
       </c>
@@ -3793,7 +3802,7 @@
       <c r="K27" s="20"/>
       <c r="L27" s="20"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B28" s="17">
         <v>26</v>
       </c>
@@ -3808,7 +3817,7 @@
       <c r="K28" s="20"/>
       <c r="L28" s="20"/>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B29" s="17">
         <v>27</v>
       </c>
@@ -3823,7 +3832,7 @@
       <c r="K29" s="20"/>
       <c r="L29" s="20"/>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B30" s="17">
         <v>28</v>
       </c>
@@ -3838,7 +3847,7 @@
       <c r="K30" s="20"/>
       <c r="L30" s="20"/>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B31" s="17">
         <v>29</v>
       </c>
@@ -3853,7 +3862,7 @@
       <c r="K31" s="20"/>
       <c r="L31" s="20"/>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B32" s="17">
         <v>30</v>
       </c>
@@ -3888,58 +3897,58 @@
   <dimension ref="B1:L33"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="H9" sqref="H7:H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="36" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="36"/>
-    <col min="3" max="3" width="28.140625" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="36" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="12" width="10.140625" style="36" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7109375" style="36"/>
+    <col min="1" max="1" width="3.26953125" style="36" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="36"/>
+    <col min="3" max="3" width="28.1796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.54296875" style="36" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="10.1796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="66" t="s">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B1" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="68" t="s">
+      <c r="F1" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="66" t="s">
+      <c r="G1" s="67" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="64" t="s">
+      <c r="I1" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="67"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="67"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B2" s="68"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="68"/>
       <c r="H2" s="35" t="s">
         <v>16</v>
       </c>
@@ -3956,7 +3965,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="255" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" ht="232" x14ac:dyDescent="0.35">
       <c r="B3" s="37">
         <v>1</v>
       </c>
@@ -3985,7 +3994,7 @@
       <c r="K3" s="42"/>
       <c r="L3" s="42"/>
     </row>
-    <row r="4" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" ht="87" x14ac:dyDescent="0.35">
       <c r="B4" s="37">
         <v>2</v>
       </c>
@@ -4014,7 +4023,7 @@
       <c r="K4" s="42"/>
       <c r="L4" s="42"/>
     </row>
-    <row r="5" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="87" x14ac:dyDescent="0.35">
       <c r="B5" s="37">
         <v>3</v>
       </c>
@@ -4043,7 +4052,7 @@
       <c r="K5" s="42"/>
       <c r="L5" s="42"/>
     </row>
-    <row r="6" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="87" x14ac:dyDescent="0.35">
       <c r="B6" s="37">
         <v>4</v>
       </c>
@@ -4072,7 +4081,7 @@
       <c r="K6" s="42"/>
       <c r="L6" s="42"/>
     </row>
-    <row r="7" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" ht="87" x14ac:dyDescent="0.35">
       <c r="B7" s="37">
         <v>5</v>
       </c>
@@ -4101,7 +4110,7 @@
       <c r="K7" s="42"/>
       <c r="L7" s="42"/>
     </row>
-    <row r="8" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" ht="87" x14ac:dyDescent="0.35">
       <c r="B8" s="37">
         <v>5</v>
       </c>
@@ -4130,7 +4139,7 @@
       <c r="K8" s="42"/>
       <c r="L8" s="42"/>
     </row>
-    <row r="9" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" ht="87" x14ac:dyDescent="0.35">
       <c r="B9" s="37">
         <v>6</v>
       </c>
@@ -4159,7 +4168,7 @@
       <c r="K9" s="42"/>
       <c r="L9" s="42"/>
     </row>
-    <row r="10" spans="2:12" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B10" s="37">
         <v>7</v>
       </c>
@@ -4188,7 +4197,7 @@
       <c r="K10" s="42"/>
       <c r="L10" s="42"/>
     </row>
-    <row r="11" spans="2:12" ht="120" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B11" s="37">
         <v>8</v>
       </c>
@@ -4217,7 +4226,7 @@
       <c r="K11" s="42"/>
       <c r="L11" s="42"/>
     </row>
-    <row r="12" spans="2:12" ht="120" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B12" s="37">
         <v>9</v>
       </c>
@@ -4246,7 +4255,7 @@
       <c r="K12" s="42"/>
       <c r="L12" s="42"/>
     </row>
-    <row r="13" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" ht="58" x14ac:dyDescent="0.35">
       <c r="B13" s="37">
         <v>10</v>
       </c>
@@ -4275,7 +4284,7 @@
       <c r="K13" s="42"/>
       <c r="L13" s="42"/>
     </row>
-    <row r="14" spans="2:12" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" ht="58" x14ac:dyDescent="0.35">
       <c r="B14" s="37">
         <v>11</v>
       </c>
@@ -4304,7 +4313,7 @@
       <c r="K14" s="42"/>
       <c r="L14" s="42"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B15" s="37">
         <v>12</v>
       </c>
@@ -4319,7 +4328,7 @@
       <c r="K15" s="42"/>
       <c r="L15" s="42"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="37">
         <v>13</v>
       </c>
@@ -4334,7 +4343,7 @@
       <c r="K16" s="42"/>
       <c r="L16" s="42"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B17" s="37">
         <v>14</v>
       </c>
@@ -4349,7 +4358,7 @@
       <c r="K17" s="42"/>
       <c r="L17" s="42"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18" s="37">
         <v>15</v>
       </c>
@@ -4364,7 +4373,7 @@
       <c r="K18" s="42"/>
       <c r="L18" s="42"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B19" s="37">
         <v>16</v>
       </c>
@@ -4379,7 +4388,7 @@
       <c r="K19" s="42"/>
       <c r="L19" s="42"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B20" s="37">
         <v>17</v>
       </c>
@@ -4394,7 +4403,7 @@
       <c r="K20" s="42"/>
       <c r="L20" s="42"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B21" s="37">
         <v>18</v>
       </c>
@@ -4409,7 +4418,7 @@
       <c r="K21" s="42"/>
       <c r="L21" s="42"/>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B22" s="37">
         <v>19</v>
       </c>
@@ -4424,7 +4433,7 @@
       <c r="K22" s="42"/>
       <c r="L22" s="42"/>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B23" s="37">
         <v>20</v>
       </c>
@@ -4439,7 +4448,7 @@
       <c r="K23" s="42"/>
       <c r="L23" s="42"/>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B24" s="37">
         <v>21</v>
       </c>
@@ -4454,7 +4463,7 @@
       <c r="K24" s="42"/>
       <c r="L24" s="42"/>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B25" s="37">
         <v>22</v>
       </c>
@@ -4469,7 +4478,7 @@
       <c r="K25" s="42"/>
       <c r="L25" s="42"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B26" s="37">
         <v>23</v>
       </c>
@@ -4484,7 +4493,7 @@
       <c r="K26" s="42"/>
       <c r="L26" s="42"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B27" s="37">
         <v>24</v>
       </c>
@@ -4499,7 +4508,7 @@
       <c r="K27" s="42"/>
       <c r="L27" s="42"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B28" s="37">
         <v>25</v>
       </c>
@@ -4514,7 +4523,7 @@
       <c r="K28" s="42"/>
       <c r="L28" s="42"/>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B29" s="37">
         <v>26</v>
       </c>
@@ -4529,7 +4538,7 @@
       <c r="K29" s="42"/>
       <c r="L29" s="42"/>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B30" s="37">
         <v>27</v>
       </c>
@@ -4544,7 +4553,7 @@
       <c r="K30" s="42"/>
       <c r="L30" s="42"/>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B31" s="37">
         <v>28</v>
       </c>
@@ -4559,7 +4568,7 @@
       <c r="K31" s="42"/>
       <c r="L31" s="42"/>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B32" s="37">
         <v>29</v>
       </c>
@@ -4574,7 +4583,7 @@
       <c r="K32" s="42"/>
       <c r="L32" s="42"/>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B33" s="37">
         <v>30</v>
       </c>
@@ -4608,59 +4617,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51635F72-9BA6-4F0C-99B9-3FC01EDB15BB}">
   <dimension ref="B1:L32"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="8"/>
-    <col min="3" max="3" width="28.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="24.140625" style="8" customWidth="1"/>
-    <col min="8" max="12" width="10.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7109375" style="8"/>
+    <col min="1" max="1" width="3.26953125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="8"/>
+    <col min="3" max="3" width="28.1796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.54296875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.81640625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="24.1796875" style="8" customWidth="1"/>
+    <col min="8" max="12" width="10.1796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.7265625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="70" t="s">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="70" t="s">
+      <c r="D1" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="70" t="s">
+      <c r="E1" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="70" t="s">
+      <c r="F1" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="70" t="s">
+      <c r="G1" s="71" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="70" t="s">
+      <c r="I1" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+    </row>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
       <c r="H2" s="7" t="s">
         <v>16</v>
       </c>
@@ -4677,7 +4686,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B3" s="9">
         <v>1</v>
       </c>
@@ -4694,13 +4703,17 @@
         <v>160</v>
       </c>
       <c r="G3" s="11"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
+      <c r="H3" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="I3" s="72" t="s">
+        <v>220</v>
+      </c>
       <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
     </row>
-    <row r="4" spans="2:12" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B4" s="9">
         <v>2</v>
       </c>
@@ -4717,13 +4730,17 @@
         <v>161</v>
       </c>
       <c r="G4" s="11"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="H4" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="I4" s="72" t="s">
+        <v>221</v>
+      </c>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
     </row>
-    <row r="5" spans="2:12" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B5" s="9">
         <v>3</v>
       </c>
@@ -4740,13 +4757,17 @@
         <v>161</v>
       </c>
       <c r="G5" s="11"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="H5" s="41" t="s">
+        <v>140</v>
+      </c>
+      <c r="I5" s="72" t="s">
+        <v>221</v>
+      </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="9">
         <v>4</v>
       </c>
@@ -4761,7 +4782,7 @@
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B7" s="9">
         <v>5</v>
       </c>
@@ -4776,7 +4797,7 @@
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B8" s="9">
         <v>6</v>
       </c>
@@ -4791,7 +4812,7 @@
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B9" s="9">
         <v>7</v>
       </c>
@@ -4806,7 +4827,7 @@
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10" s="9">
         <v>8</v>
       </c>
@@ -4821,7 +4842,7 @@
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B11" s="9">
         <v>9</v>
       </c>
@@ -4836,7 +4857,7 @@
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B12" s="9">
         <v>10</v>
       </c>
@@ -4851,7 +4872,7 @@
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B13" s="9">
         <v>11</v>
       </c>
@@ -4866,7 +4887,7 @@
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B14" s="9">
         <v>12</v>
       </c>
@@ -4881,7 +4902,7 @@
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B15" s="9">
         <v>13</v>
       </c>
@@ -4896,7 +4917,7 @@
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B16" s="9">
         <v>14</v>
       </c>
@@ -4911,7 +4932,7 @@
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B17" s="9">
         <v>15</v>
       </c>
@@ -4926,7 +4947,7 @@
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B18" s="9">
         <v>16</v>
       </c>
@@ -4941,7 +4962,7 @@
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B19" s="9">
         <v>17</v>
       </c>
@@ -4956,7 +4977,7 @@
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B20" s="9">
         <v>18</v>
       </c>
@@ -4971,7 +4992,7 @@
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B21" s="9">
         <v>19</v>
       </c>
@@ -4986,7 +5007,7 @@
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B22" s="9">
         <v>20</v>
       </c>
@@ -5001,7 +5022,7 @@
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B23" s="9">
         <v>21</v>
       </c>
@@ -5016,7 +5037,7 @@
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B24" s="9">
         <v>22</v>
       </c>
@@ -5031,7 +5052,7 @@
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B25" s="9">
         <v>23</v>
       </c>
@@ -5046,7 +5067,7 @@
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B26" s="9">
         <v>24</v>
       </c>
@@ -5061,7 +5082,7 @@
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B27" s="9">
         <v>25</v>
       </c>
@@ -5076,7 +5097,7 @@
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B28" s="9">
         <v>26</v>
       </c>
@@ -5091,7 +5112,7 @@
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B29" s="9">
         <v>27</v>
       </c>
@@ -5106,7 +5127,7 @@
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B30" s="9">
         <v>28</v>
       </c>
@@ -5121,7 +5142,7 @@
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B31" s="9">
         <v>29</v>
       </c>
@@ -5136,7 +5157,7 @@
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B32" s="9">
         <v>30</v>
       </c>

</xml_diff>